<commit_message>
add json-feature and set time format
</commit_message>
<xml_diff>
--- a/file.xlsx
+++ b/file.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="17400" windowHeight="12972" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="17400" windowHeight="12972"/>
   </bookViews>
   <sheets>
     <sheet name="1 курс" sheetId="2" r:id="rId1"/>
@@ -5462,6 +5462,30 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5549,13 +5573,13 @@
     <xf numFmtId="0" fontId="18" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -5564,46 +5588,22 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5909,8 +5909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U57"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="37.6640625" defaultRowHeight="30" customHeight="1"/>
@@ -5923,20 +5923,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="1" customFormat="1" ht="45" customHeight="1">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="71" t="s">
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="75" t="s">
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="83" t="s">
         <v>351</v>
       </c>
-      <c r="H1" s="75"/>
+      <c r="H1" s="83"/>
       <c r="I1" s="30"/>
       <c r="J1" s="30"/>
       <c r="K1" s="30"/>
@@ -5950,18 +5950,18 @@
       <c r="S1" s="32"/>
     </row>
     <row r="2" spans="1:21" s="1" customFormat="1" ht="43.2" customHeight="1">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="74" t="s">
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
       <c r="I2" s="31"/>
       <c r="J2" s="31"/>
       <c r="K2" s="31"/>
@@ -6036,35 +6036,35 @@
       <c r="U3" s="5"/>
     </row>
     <row r="4" spans="1:21" ht="76.05" customHeight="1">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="62" t="s">
         <v>102</v>
       </c>
       <c r="B4" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="C4" s="62" t="s">
+      <c r="C4" s="70" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="63"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="62" t="s">
+      <c r="D4" s="71"/>
+      <c r="E4" s="72"/>
+      <c r="F4" s="70" t="s">
         <v>84</v>
       </c>
-      <c r="G4" s="63"/>
-      <c r="H4" s="64"/>
-      <c r="I4" s="62" t="s">
+      <c r="G4" s="71"/>
+      <c r="H4" s="72"/>
+      <c r="I4" s="70" t="s">
         <v>85</v>
       </c>
-      <c r="J4" s="63"/>
-      <c r="K4" s="64"/>
-      <c r="L4" s="62" t="s">
+      <c r="J4" s="71"/>
+      <c r="K4" s="72"/>
+      <c r="L4" s="70" t="s">
         <v>86</v>
       </c>
-      <c r="M4" s="64"/>
-      <c r="N4" s="67" t="s">
+      <c r="M4" s="72"/>
+      <c r="N4" s="75" t="s">
         <v>320</v>
       </c>
-      <c r="O4" s="68"/>
+      <c r="O4" s="76"/>
       <c r="P4" s="18"/>
       <c r="Q4" s="18"/>
       <c r="R4" s="18"/>
@@ -6073,46 +6073,46 @@
       <c r="U4" s="5"/>
     </row>
     <row r="5" spans="1:21" ht="75.599999999999994" customHeight="1">
-      <c r="A5" s="55"/>
+      <c r="A5" s="63"/>
       <c r="B5" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="C5" s="57" t="s">
+      <c r="C5" s="65" t="s">
         <v>88</v>
       </c>
-      <c r="D5" s="58"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="57" t="s">
+      <c r="D5" s="66"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="65" t="s">
         <v>89</v>
       </c>
-      <c r="G5" s="58"/>
-      <c r="H5" s="59"/>
-      <c r="I5" s="57" t="s">
+      <c r="G5" s="66"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="65" t="s">
         <v>90</v>
       </c>
-      <c r="J5" s="58"/>
-      <c r="K5" s="59"/>
-      <c r="L5" s="57" t="s">
+      <c r="J5" s="66"/>
+      <c r="K5" s="67"/>
+      <c r="L5" s="65" t="s">
         <v>91</v>
       </c>
-      <c r="M5" s="59"/>
-      <c r="N5" s="60" t="s">
+      <c r="M5" s="67"/>
+      <c r="N5" s="68" t="s">
         <v>92</v>
       </c>
-      <c r="O5" s="61"/>
-      <c r="P5" s="60" t="s">
+      <c r="O5" s="69"/>
+      <c r="P5" s="68" t="s">
         <v>93</v>
       </c>
-      <c r="Q5" s="61"/>
-      <c r="R5" s="60" t="s">
+      <c r="Q5" s="69"/>
+      <c r="R5" s="68" t="s">
         <v>94</v>
       </c>
-      <c r="S5" s="61"/>
+      <c r="S5" s="69"/>
       <c r="T5" s="5"/>
       <c r="U5" s="5"/>
     </row>
     <row r="6" spans="1:21" ht="85.8" customHeight="1">
-      <c r="A6" s="55"/>
+      <c r="A6" s="63"/>
       <c r="B6" s="10" t="s">
         <v>100</v>
       </c>
@@ -6121,72 +6121,72 @@
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
-      <c r="F6" s="57" t="s">
+      <c r="F6" s="65" t="s">
         <v>97</v>
       </c>
-      <c r="G6" s="58"/>
-      <c r="H6" s="59"/>
-      <c r="I6" s="57" t="s">
+      <c r="G6" s="66"/>
+      <c r="H6" s="67"/>
+      <c r="I6" s="65" t="s">
         <v>90</v>
       </c>
-      <c r="J6" s="58"/>
-      <c r="K6" s="59"/>
-      <c r="L6" s="57" t="s">
+      <c r="J6" s="66"/>
+      <c r="K6" s="67"/>
+      <c r="L6" s="65" t="s">
         <v>98</v>
       </c>
-      <c r="M6" s="59"/>
+      <c r="M6" s="67"/>
       <c r="N6" s="9"/>
       <c r="O6" s="9"/>
-      <c r="P6" s="60" t="s">
+      <c r="P6" s="68" t="s">
         <v>99</v>
       </c>
-      <c r="Q6" s="61"/>
-      <c r="R6" s="60" t="s">
+      <c r="Q6" s="69"/>
+      <c r="R6" s="68" t="s">
         <v>94</v>
       </c>
-      <c r="S6" s="61"/>
+      <c r="S6" s="69"/>
       <c r="T6" s="5"/>
       <c r="U6" s="5"/>
     </row>
     <row r="7" spans="1:21" ht="123.6" customHeight="1" thickBot="1">
-      <c r="A7" s="56"/>
+      <c r="A7" s="64"/>
       <c r="B7" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="C7" s="51" t="s">
+      <c r="C7" s="59" t="s">
         <v>329</v>
       </c>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="51" t="s">
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="59" t="s">
         <v>329</v>
       </c>
-      <c r="G7" s="53"/>
-      <c r="H7" s="53"/>
-      <c r="I7" s="51" t="s">
+      <c r="G7" s="61"/>
+      <c r="H7" s="61"/>
+      <c r="I7" s="59" t="s">
         <v>329</v>
       </c>
-      <c r="J7" s="53"/>
-      <c r="K7" s="53"/>
-      <c r="L7" s="51" t="s">
+      <c r="J7" s="61"/>
+      <c r="K7" s="61"/>
+      <c r="L7" s="59" t="s">
         <v>329</v>
       </c>
-      <c r="M7" s="53"/>
-      <c r="N7" s="53"/>
-      <c r="O7" s="53"/>
-      <c r="P7" s="51" t="s">
+      <c r="M7" s="61"/>
+      <c r="N7" s="61"/>
+      <c r="O7" s="61"/>
+      <c r="P7" s="59" t="s">
         <v>329</v>
       </c>
-      <c r="Q7" s="52"/>
-      <c r="R7" s="51" t="s">
+      <c r="Q7" s="60"/>
+      <c r="R7" s="59" t="s">
         <v>330</v>
       </c>
-      <c r="S7" s="52"/>
+      <c r="S7" s="60"/>
       <c r="T7" s="5"/>
       <c r="U7" s="5"/>
     </row>
     <row r="8" spans="1:21" ht="94.2">
-      <c r="A8" s="54" t="s">
+      <c r="A8" s="62" t="s">
         <v>123</v>
       </c>
       <c r="B8" s="17" t="s">
@@ -6207,10 +6207,10 @@
       <c r="I8" s="20"/>
       <c r="J8" s="20"/>
       <c r="K8" s="20"/>
-      <c r="L8" s="62" t="s">
+      <c r="L8" s="70" t="s">
         <v>324</v>
       </c>
-      <c r="M8" s="64"/>
+      <c r="M8" s="72"/>
       <c r="N8" s="18"/>
       <c r="O8" s="18"/>
       <c r="P8" s="18"/>
@@ -6221,7 +6221,7 @@
       <c r="U8" s="5"/>
     </row>
     <row r="9" spans="1:21" ht="141" customHeight="1">
-      <c r="A9" s="55"/>
+      <c r="A9" s="63"/>
       <c r="B9" s="10" t="s">
         <v>95</v>
       </c>
@@ -6244,25 +6244,25 @@
       </c>
       <c r="J9" s="13"/>
       <c r="K9" s="13"/>
-      <c r="L9" s="57" t="s">
+      <c r="L9" s="65" t="s">
         <v>108</v>
       </c>
-      <c r="M9" s="59"/>
+      <c r="M9" s="67"/>
       <c r="N9" s="9"/>
       <c r="O9" s="9"/>
-      <c r="P9" s="60" t="s">
+      <c r="P9" s="68" t="s">
         <v>93</v>
       </c>
-      <c r="Q9" s="61"/>
-      <c r="R9" s="60" t="s">
+      <c r="Q9" s="69"/>
+      <c r="R9" s="68" t="s">
         <v>109</v>
       </c>
-      <c r="S9" s="61"/>
+      <c r="S9" s="69"/>
       <c r="T9" s="5"/>
       <c r="U9" s="5"/>
     </row>
     <row r="10" spans="1:21" ht="112.8">
-      <c r="A10" s="55"/>
+      <c r="A10" s="63"/>
       <c r="B10" s="10" t="s">
         <v>100</v>
       </c>
@@ -6285,27 +6285,27 @@
       </c>
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
-      <c r="L10" s="57" t="s">
+      <c r="L10" s="65" t="s">
         <v>113</v>
       </c>
-      <c r="M10" s="59"/>
-      <c r="N10" s="60" t="s">
+      <c r="M10" s="67"/>
+      <c r="N10" s="68" t="s">
         <v>114</v>
       </c>
-      <c r="O10" s="61"/>
-      <c r="P10" s="60" t="s">
+      <c r="O10" s="69"/>
+      <c r="P10" s="68" t="s">
         <v>99</v>
       </c>
-      <c r="Q10" s="61"/>
-      <c r="R10" s="60" t="s">
+      <c r="Q10" s="69"/>
+      <c r="R10" s="68" t="s">
         <v>115</v>
       </c>
-      <c r="S10" s="61"/>
+      <c r="S10" s="69"/>
       <c r="T10" s="5"/>
       <c r="U10" s="5"/>
     </row>
     <row r="11" spans="1:21" ht="171" customHeight="1">
-      <c r="A11" s="55"/>
+      <c r="A11" s="63"/>
       <c r="B11" s="10" t="s">
         <v>101</v>
       </c>
@@ -6332,25 +6332,25 @@
       <c r="K11" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="L11" s="57" t="s">
+      <c r="L11" s="65" t="s">
         <v>113</v>
       </c>
-      <c r="M11" s="59"/>
-      <c r="N11" s="60" t="s">
+      <c r="M11" s="67"/>
+      <c r="N11" s="68" t="s">
         <v>120</v>
       </c>
-      <c r="O11" s="61"/>
+      <c r="O11" s="69"/>
       <c r="P11" s="9"/>
       <c r="Q11" s="9"/>
-      <c r="R11" s="60" t="s">
+      <c r="R11" s="68" t="s">
         <v>121</v>
       </c>
-      <c r="S11" s="61"/>
+      <c r="S11" s="69"/>
       <c r="T11" s="5"/>
       <c r="U11" s="5"/>
     </row>
     <row r="12" spans="1:21" ht="87.6" customHeight="1" thickBot="1">
-      <c r="A12" s="56"/>
+      <c r="A12" s="64"/>
       <c r="B12" s="19" t="s">
         <v>308</v>
       </c>
@@ -6373,10 +6373,10 @@
       </c>
       <c r="L12" s="22"/>
       <c r="M12" s="22"/>
-      <c r="N12" s="65" t="s">
+      <c r="N12" s="73" t="s">
         <v>120</v>
       </c>
-      <c r="O12" s="66"/>
+      <c r="O12" s="74"/>
       <c r="P12" s="23"/>
       <c r="Q12" s="23"/>
       <c r="R12" s="23"/>
@@ -6385,7 +6385,7 @@
       <c r="U12" s="5"/>
     </row>
     <row r="13" spans="1:21" ht="106.8" customHeight="1">
-      <c r="A13" s="54" t="s">
+      <c r="A13" s="62" t="s">
         <v>145</v>
       </c>
       <c r="B13" s="17" t="s">
@@ -6410,33 +6410,33 @@
       </c>
       <c r="L13" s="20"/>
       <c r="M13" s="20"/>
-      <c r="N13" s="67" t="s">
+      <c r="N13" s="75" t="s">
         <v>126</v>
       </c>
-      <c r="O13" s="68"/>
+      <c r="O13" s="76"/>
       <c r="P13" s="18" t="s">
         <v>127</v>
       </c>
       <c r="Q13" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="R13" s="67" t="s">
+      <c r="R13" s="75" t="s">
         <v>129</v>
       </c>
-      <c r="S13" s="68"/>
+      <c r="S13" s="76"/>
       <c r="T13" s="5"/>
       <c r="U13" s="5"/>
     </row>
     <row r="14" spans="1:21" ht="132.6">
-      <c r="A14" s="55"/>
+      <c r="A14" s="63"/>
       <c r="B14" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="C14" s="57" t="s">
+      <c r="C14" s="65" t="s">
         <v>130</v>
       </c>
-      <c r="D14" s="58"/>
-      <c r="E14" s="59"/>
+      <c r="D14" s="66"/>
+      <c r="E14" s="67"/>
       <c r="F14" s="13" t="s">
         <v>131</v>
       </c>
@@ -6451,37 +6451,37 @@
       <c r="K14" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="L14" s="57" t="s">
+      <c r="L14" s="65" t="s">
         <v>84</v>
       </c>
-      <c r="M14" s="59"/>
-      <c r="N14" s="60" t="s">
+      <c r="M14" s="67"/>
+      <c r="N14" s="68" t="s">
         <v>133</v>
       </c>
-      <c r="O14" s="61"/>
+      <c r="O14" s="69"/>
       <c r="P14" s="9" t="s">
         <v>127</v>
       </c>
       <c r="Q14" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="R14" s="60" t="s">
+      <c r="R14" s="68" t="s">
         <v>134</v>
       </c>
-      <c r="S14" s="61"/>
+      <c r="S14" s="69"/>
       <c r="T14" s="5"/>
       <c r="U14" s="5"/>
     </row>
     <row r="15" spans="1:21" ht="102" customHeight="1">
-      <c r="A15" s="55"/>
+      <c r="A15" s="63"/>
       <c r="B15" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="C15" s="57" t="s">
+      <c r="C15" s="65" t="s">
         <v>135</v>
       </c>
-      <c r="D15" s="58"/>
-      <c r="E15" s="59"/>
+      <c r="D15" s="66"/>
+      <c r="E15" s="67"/>
       <c r="F15" s="13" t="s">
         <v>316</v>
       </c>
@@ -6498,14 +6498,14 @@
       <c r="K15" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="L15" s="57" t="s">
+      <c r="L15" s="65" t="s">
         <v>138</v>
       </c>
-      <c r="M15" s="59"/>
-      <c r="N15" s="60" t="s">
+      <c r="M15" s="67"/>
+      <c r="N15" s="68" t="s">
         <v>323</v>
       </c>
-      <c r="O15" s="61"/>
+      <c r="O15" s="69"/>
       <c r="P15" s="9" t="s">
         <v>139</v>
       </c>
@@ -6520,15 +6520,15 @@
       <c r="U15" s="5"/>
     </row>
     <row r="16" spans="1:21" ht="108.6" customHeight="1">
-      <c r="A16" s="55"/>
+      <c r="A16" s="63"/>
       <c r="B16" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="C16" s="57" t="s">
+      <c r="C16" s="65" t="s">
         <v>142</v>
       </c>
-      <c r="D16" s="58"/>
-      <c r="E16" s="59"/>
+      <c r="D16" s="66"/>
+      <c r="E16" s="67"/>
       <c r="F16" s="13" t="s">
         <v>316</v>
       </c>
@@ -6545,10 +6545,10 @@
       </c>
       <c r="L16" s="13"/>
       <c r="M16" s="13"/>
-      <c r="N16" s="60" t="s">
+      <c r="N16" s="68" t="s">
         <v>323</v>
       </c>
-      <c r="O16" s="61"/>
+      <c r="O16" s="69"/>
       <c r="P16" s="9" t="s">
         <v>139</v>
       </c>
@@ -6563,7 +6563,7 @@
       <c r="U16" s="5"/>
     </row>
     <row r="17" spans="1:21" ht="91.8" customHeight="1">
-      <c r="A17" s="55"/>
+      <c r="A17" s="63"/>
       <c r="B17" s="10" t="s">
         <v>122</v>
       </c>
@@ -6596,7 +6596,7 @@
       <c r="U17" s="5"/>
     </row>
     <row r="18" spans="1:21" ht="111" customHeight="1" thickBot="1">
-      <c r="A18" s="56"/>
+      <c r="A18" s="64"/>
       <c r="B18" s="19" t="s">
         <v>144</v>
       </c>
@@ -6625,7 +6625,7 @@
       <c r="U18" s="5"/>
     </row>
     <row r="19" spans="1:21" ht="76.05" customHeight="1">
-      <c r="A19" s="54" t="s">
+      <c r="A19" s="62" t="s">
         <v>160</v>
       </c>
       <c r="B19" s="17" t="s">
@@ -6639,26 +6639,26 @@
       </c>
       <c r="G19" s="20"/>
       <c r="H19" s="20"/>
-      <c r="I19" s="62" t="s">
+      <c r="I19" s="70" t="s">
         <v>146</v>
       </c>
-      <c r="J19" s="63"/>
-      <c r="K19" s="64"/>
+      <c r="J19" s="71"/>
+      <c r="K19" s="72"/>
       <c r="L19" s="20"/>
       <c r="M19" s="20"/>
       <c r="N19" s="18"/>
       <c r="O19" s="18"/>
       <c r="P19" s="18"/>
       <c r="Q19" s="18"/>
-      <c r="R19" s="60" t="s">
+      <c r="R19" s="68" t="s">
         <v>159</v>
       </c>
-      <c r="S19" s="61"/>
+      <c r="S19" s="69"/>
       <c r="T19" s="5"/>
       <c r="U19" s="5"/>
     </row>
     <row r="20" spans="1:21" ht="75.599999999999994">
-      <c r="A20" s="55"/>
+      <c r="A20" s="63"/>
       <c r="B20" s="10" t="s">
         <v>95</v>
       </c>
@@ -6678,28 +6678,28 @@
       <c r="H20" s="13" t="s">
         <v>344</v>
       </c>
-      <c r="I20" s="57" t="s">
+      <c r="I20" s="65" t="s">
         <v>85</v>
       </c>
-      <c r="J20" s="58"/>
-      <c r="K20" s="59"/>
+      <c r="J20" s="66"/>
+      <c r="K20" s="67"/>
       <c r="L20" s="13"/>
       <c r="M20" s="13"/>
-      <c r="N20" s="60" t="s">
+      <c r="N20" s="68" t="s">
         <v>149</v>
       </c>
-      <c r="O20" s="61"/>
+      <c r="O20" s="69"/>
       <c r="P20" s="9"/>
       <c r="Q20" s="9"/>
-      <c r="R20" s="60" t="s">
+      <c r="R20" s="68" t="s">
         <v>150</v>
       </c>
-      <c r="S20" s="61"/>
+      <c r="S20" s="69"/>
       <c r="T20" s="5"/>
       <c r="U20" s="5"/>
     </row>
     <row r="21" spans="1:21" ht="75.599999999999994">
-      <c r="A21" s="55"/>
+      <c r="A21" s="63"/>
       <c r="B21" s="10" t="s">
         <v>100</v>
       </c>
@@ -6719,32 +6719,32 @@
       <c r="H21" s="13" t="s">
         <v>345</v>
       </c>
-      <c r="I21" s="57" t="s">
+      <c r="I21" s="65" t="s">
         <v>151</v>
       </c>
-      <c r="J21" s="58"/>
-      <c r="K21" s="59"/>
+      <c r="J21" s="66"/>
+      <c r="K21" s="67"/>
       <c r="L21" s="13"/>
       <c r="M21" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="N21" s="60" t="s">
+      <c r="N21" s="68" t="s">
         <v>149</v>
       </c>
-      <c r="O21" s="61"/>
-      <c r="P21" s="60" t="s">
+      <c r="O21" s="69"/>
+      <c r="P21" s="68" t="s">
         <v>153</v>
       </c>
-      <c r="Q21" s="61"/>
-      <c r="R21" s="60" t="s">
+      <c r="Q21" s="69"/>
+      <c r="R21" s="68" t="s">
         <v>154</v>
       </c>
-      <c r="S21" s="61"/>
+      <c r="S21" s="69"/>
       <c r="T21" s="5"/>
       <c r="U21" s="5"/>
     </row>
     <row r="22" spans="1:21" ht="93" customHeight="1">
-      <c r="A22" s="55"/>
+      <c r="A22" s="63"/>
       <c r="B22" s="10" t="s">
         <v>101</v>
       </c>
@@ -6762,32 +6762,32 @@
       <c r="H22" s="13" t="s">
         <v>346</v>
       </c>
-      <c r="I22" s="57" t="s">
+      <c r="I22" s="65" t="s">
         <v>151</v>
       </c>
-      <c r="J22" s="58"/>
-      <c r="K22" s="59"/>
-      <c r="L22" s="57" t="s">
+      <c r="J22" s="66"/>
+      <c r="K22" s="67"/>
+      <c r="L22" s="65" t="s">
         <v>157</v>
       </c>
-      <c r="M22" s="59"/>
+      <c r="M22" s="67"/>
       <c r="N22" s="9" t="s">
         <v>158</v>
       </c>
       <c r="O22" s="9"/>
-      <c r="P22" s="60" t="s">
+      <c r="P22" s="68" t="s">
         <v>153</v>
       </c>
-      <c r="Q22" s="61"/>
-      <c r="R22" s="60" t="s">
+      <c r="Q22" s="69"/>
+      <c r="R22" s="68" t="s">
         <v>154</v>
       </c>
-      <c r="S22" s="61"/>
+      <c r="S22" s="69"/>
       <c r="T22" s="5"/>
       <c r="U22" s="5"/>
     </row>
     <row r="23" spans="1:21" ht="70.8" customHeight="1">
-      <c r="A23" s="55"/>
+      <c r="A23" s="63"/>
       <c r="B23" s="10" t="s">
         <v>308</v>
       </c>
@@ -6802,23 +6802,23 @@
       <c r="I23" s="13"/>
       <c r="J23" s="13"/>
       <c r="K23" s="13"/>
-      <c r="L23" s="57" t="s">
+      <c r="L23" s="65" t="s">
         <v>157</v>
       </c>
-      <c r="M23" s="59"/>
+      <c r="M23" s="67"/>
       <c r="N23" s="9" t="s">
         <v>158</v>
       </c>
       <c r="O23" s="9"/>
       <c r="P23" s="9"/>
       <c r="Q23" s="9"/>
-      <c r="R23" s="60"/>
-      <c r="S23" s="61"/>
+      <c r="R23" s="68"/>
+      <c r="S23" s="69"/>
       <c r="T23" s="5"/>
       <c r="U23" s="5"/>
     </row>
     <row r="24" spans="1:21" ht="92.4" customHeight="1" thickBot="1">
-      <c r="A24" s="56"/>
+      <c r="A24" s="64"/>
       <c r="B24" s="19" t="s">
         <v>144</v>
       </c>
@@ -6832,10 +6832,10 @@
       <c r="J24" s="22"/>
       <c r="K24" s="22"/>
       <c r="L24" s="22"/>
-      <c r="M24" s="22" t="s">
+      <c r="M24" s="22"/>
+      <c r="N24" s="47" t="s">
         <v>143</v>
       </c>
-      <c r="N24" s="23"/>
       <c r="O24" s="23"/>
       <c r="P24" s="23"/>
       <c r="Q24" s="23"/>
@@ -6845,7 +6845,7 @@
       <c r="U24" s="5"/>
     </row>
     <row r="25" spans="1:21" ht="74.400000000000006" customHeight="1">
-      <c r="A25" s="54" t="s">
+      <c r="A25" s="62" t="s">
         <v>173</v>
       </c>
       <c r="B25" s="17" t="s">
@@ -6878,7 +6878,7 @@
       <c r="U25" s="5"/>
     </row>
     <row r="26" spans="1:21" ht="145.80000000000001" customHeight="1">
-      <c r="A26" s="55"/>
+      <c r="A26" s="63"/>
       <c r="B26" s="10" t="s">
         <v>95</v>
       </c>
@@ -6890,11 +6890,11 @@
       </c>
       <c r="G26" s="13"/>
       <c r="H26" s="13"/>
-      <c r="I26" s="57" t="s">
+      <c r="I26" s="65" t="s">
         <v>146</v>
       </c>
-      <c r="J26" s="58"/>
-      <c r="K26" s="59"/>
+      <c r="J26" s="66"/>
+      <c r="K26" s="67"/>
       <c r="L26" s="13"/>
       <c r="M26" s="13" t="s">
         <v>161</v>
@@ -6915,15 +6915,15 @@
       <c r="U26" s="5"/>
     </row>
     <row r="27" spans="1:21" ht="88.8" customHeight="1">
-      <c r="A27" s="55"/>
+      <c r="A27" s="63"/>
       <c r="B27" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="C27" s="57" t="s">
+      <c r="C27" s="65" t="s">
         <v>88</v>
       </c>
-      <c r="D27" s="58"/>
-      <c r="E27" s="59"/>
+      <c r="D27" s="66"/>
+      <c r="E27" s="67"/>
       <c r="F27" s="13" t="s">
         <v>163</v>
       </c>
@@ -6933,11 +6933,11 @@
       <c r="H27" s="13" t="s">
         <v>339</v>
       </c>
-      <c r="I27" s="57" t="s">
+      <c r="I27" s="65" t="s">
         <v>166</v>
       </c>
-      <c r="J27" s="58"/>
-      <c r="K27" s="59"/>
+      <c r="J27" s="66"/>
+      <c r="K27" s="67"/>
       <c r="L27" s="13" t="s">
         <v>167</v>
       </c>
@@ -6962,15 +6962,15 @@
       <c r="U27" s="5"/>
     </row>
     <row r="28" spans="1:21" ht="93.6" customHeight="1">
-      <c r="A28" s="55"/>
+      <c r="A28" s="63"/>
       <c r="B28" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="C28" s="57" t="s">
+      <c r="C28" s="65" t="s">
         <v>170</v>
       </c>
-      <c r="D28" s="58"/>
-      <c r="E28" s="59"/>
+      <c r="D28" s="66"/>
+      <c r="E28" s="67"/>
       <c r="F28" s="13" t="s">
         <v>171</v>
       </c>
@@ -6980,11 +6980,11 @@
       <c r="H28" s="13" t="s">
         <v>339</v>
       </c>
-      <c r="I28" s="57" t="s">
+      <c r="I28" s="65" t="s">
         <v>166</v>
       </c>
-      <c r="J28" s="58"/>
-      <c r="K28" s="59"/>
+      <c r="J28" s="66"/>
+      <c r="K28" s="67"/>
       <c r="L28" s="13" t="s">
         <v>167</v>
       </c>
@@ -7009,15 +7009,15 @@
       <c r="U28" s="5"/>
     </row>
     <row r="29" spans="1:21" ht="93.6" customHeight="1">
-      <c r="A29" s="55"/>
+      <c r="A29" s="63"/>
       <c r="B29" s="10" t="s">
         <v>308</v>
       </c>
-      <c r="C29" s="48" t="s">
+      <c r="C29" s="56" t="s">
         <v>170</v>
       </c>
-      <c r="D29" s="49"/>
-      <c r="E29" s="50"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="58"/>
       <c r="F29" s="43"/>
       <c r="G29" s="43" t="s">
         <v>172</v>
@@ -7040,13 +7040,13 @@
       <c r="U29" s="5"/>
     </row>
     <row r="30" spans="1:21" ht="71.400000000000006" customHeight="1" thickBot="1">
-      <c r="A30" s="56"/>
+      <c r="A30" s="64"/>
       <c r="B30" s="19" t="s">
         <v>309</v>
       </c>
-      <c r="C30" s="51"/>
-      <c r="D30" s="53"/>
-      <c r="E30" s="52"/>
+      <c r="C30" s="59"/>
+      <c r="D30" s="61"/>
+      <c r="E30" s="60"/>
       <c r="F30" s="22"/>
       <c r="G30" s="22"/>
       <c r="H30" s="22" t="s">
@@ -7728,20 +7728,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1" ht="45" customHeight="1">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="71" t="s">
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="75" t="s">
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="83" t="s">
         <v>351</v>
       </c>
-      <c r="H1" s="75"/>
+      <c r="H1" s="83"/>
       <c r="I1" s="30"/>
       <c r="J1" s="30"/>
       <c r="K1" s="30"/>
@@ -7750,18 +7750,18 @@
       <c r="N1" s="30"/>
     </row>
     <row r="2" spans="1:14" s="1" customFormat="1" ht="47.4" customHeight="1">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="74" t="s">
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
       <c r="I2" s="31"/>
       <c r="J2" s="31"/>
       <c r="K2" s="31"/>
@@ -7814,7 +7814,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="99.6" customHeight="1">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="62" t="s">
         <v>102</v>
       </c>
       <c r="B4" s="17" t="s">
@@ -7826,10 +7826,10 @@
       <c r="D4" s="20" t="s">
         <v>347</v>
       </c>
-      <c r="E4" s="62" t="s">
+      <c r="E4" s="70" t="s">
         <v>177</v>
       </c>
-      <c r="F4" s="64"/>
+      <c r="F4" s="72"/>
       <c r="G4" s="20"/>
       <c r="H4" s="20" t="s">
         <v>181</v>
@@ -7840,13 +7840,13 @@
       <c r="J4" s="20"/>
       <c r="K4" s="20"/>
       <c r="L4" s="20"/>
-      <c r="M4" s="62" t="s">
+      <c r="M4" s="70" t="s">
         <v>179</v>
       </c>
-      <c r="N4" s="64"/>
+      <c r="N4" s="72"/>
     </row>
     <row r="5" spans="1:14" ht="99.6" customHeight="1">
-      <c r="A5" s="55"/>
+      <c r="A5" s="63"/>
       <c r="B5" s="10" t="s">
         <v>95</v>
       </c>
@@ -7856,10 +7856,10 @@
       <c r="D5" s="13" t="s">
         <v>347</v>
       </c>
-      <c r="E5" s="57" t="s">
+      <c r="E5" s="65" t="s">
         <v>177</v>
       </c>
-      <c r="F5" s="59"/>
+      <c r="F5" s="67"/>
       <c r="G5" s="13"/>
       <c r="H5" s="13" t="s">
         <v>181</v>
@@ -7870,20 +7870,20 @@
       <c r="J5" s="13"/>
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
-      <c r="M5" s="57" t="s">
+      <c r="M5" s="65" t="s">
         <v>179</v>
       </c>
-      <c r="N5" s="59"/>
+      <c r="N5" s="67"/>
     </row>
     <row r="6" spans="1:14" ht="91.2" customHeight="1">
-      <c r="A6" s="55"/>
+      <c r="A6" s="63"/>
       <c r="B6" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="C6" s="57" t="s">
+      <c r="C6" s="65" t="s">
         <v>182</v>
       </c>
-      <c r="D6" s="59"/>
+      <c r="D6" s="67"/>
       <c r="E6" s="13" t="s">
         <v>348</v>
       </c>
@@ -7906,7 +7906,7 @@
       <c r="N6" s="9"/>
     </row>
     <row r="7" spans="1:14" ht="94.8" customHeight="1">
-      <c r="A7" s="55"/>
+      <c r="A7" s="63"/>
       <c r="B7" s="10" t="s">
         <v>101</v>
       </c>
@@ -7934,7 +7934,7 @@
       <c r="N7" s="9"/>
     </row>
     <row r="8" spans="1:14" ht="97.8" customHeight="1" thickBot="1">
-      <c r="A8" s="56"/>
+      <c r="A8" s="64"/>
       <c r="B8" s="19" t="s">
         <v>308</v>
       </c>
@@ -7954,7 +7954,7 @@
       <c r="N8" s="23"/>
     </row>
     <row r="9" spans="1:14" ht="76.05" customHeight="1">
-      <c r="A9" s="54" t="s">
+      <c r="A9" s="62" t="s">
         <v>123</v>
       </c>
       <c r="B9" s="17" t="s">
@@ -7962,106 +7962,106 @@
       </c>
       <c r="C9" s="20"/>
       <c r="D9" s="20"/>
-      <c r="E9" s="62" t="s">
+      <c r="E9" s="70" t="s">
         <v>190</v>
       </c>
-      <c r="F9" s="64"/>
+      <c r="F9" s="72"/>
       <c r="G9" s="20"/>
       <c r="H9" s="20"/>
       <c r="I9" s="20"/>
       <c r="J9" s="20"/>
       <c r="K9" s="20"/>
       <c r="L9" s="20"/>
-      <c r="M9" s="62" t="s">
+      <c r="M9" s="70" t="s">
         <v>191</v>
       </c>
-      <c r="N9" s="64"/>
+      <c r="N9" s="72"/>
     </row>
     <row r="10" spans="1:14" ht="75.599999999999994" customHeight="1">
-      <c r="A10" s="55"/>
+      <c r="A10" s="63"/>
       <c r="B10" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="C10" s="57" t="s">
+      <c r="C10" s="65" t="s">
         <v>192</v>
       </c>
-      <c r="D10" s="59"/>
-      <c r="E10" s="57" t="s">
+      <c r="D10" s="67"/>
+      <c r="E10" s="65" t="s">
         <v>190</v>
       </c>
-      <c r="F10" s="59"/>
-      <c r="G10" s="57" t="s">
+      <c r="F10" s="67"/>
+      <c r="G10" s="65" t="s">
         <v>193</v>
       </c>
-      <c r="H10" s="59"/>
+      <c r="H10" s="67"/>
       <c r="I10" s="13"/>
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
-      <c r="M10" s="57" t="s">
+      <c r="M10" s="65" t="s">
         <v>191</v>
       </c>
-      <c r="N10" s="59"/>
+      <c r="N10" s="67"/>
     </row>
     <row r="11" spans="1:14" ht="75.599999999999994" customHeight="1">
-      <c r="A11" s="55"/>
+      <c r="A11" s="63"/>
       <c r="B11" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="C11" s="57" t="s">
+      <c r="C11" s="65" t="s">
         <v>194</v>
       </c>
-      <c r="D11" s="59"/>
-      <c r="E11" s="57" t="s">
+      <c r="D11" s="67"/>
+      <c r="E11" s="65" t="s">
         <v>195</v>
       </c>
-      <c r="F11" s="59"/>
-      <c r="G11" s="57" t="s">
+      <c r="F11" s="67"/>
+      <c r="G11" s="65" t="s">
         <v>193</v>
       </c>
-      <c r="H11" s="59"/>
+      <c r="H11" s="67"/>
       <c r="I11" s="13"/>
       <c r="J11" s="13"/>
       <c r="K11" s="13"/>
       <c r="L11" s="13"/>
-      <c r="M11" s="57" t="s">
+      <c r="M11" s="65" t="s">
         <v>321</v>
       </c>
-      <c r="N11" s="59"/>
+      <c r="N11" s="67"/>
     </row>
     <row r="12" spans="1:14" ht="75.599999999999994" customHeight="1">
-      <c r="A12" s="55"/>
+      <c r="A12" s="63"/>
       <c r="B12" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="C12" s="57" t="s">
+      <c r="C12" s="65" t="s">
         <v>196</v>
       </c>
-      <c r="D12" s="59"/>
-      <c r="E12" s="57" t="s">
+      <c r="D12" s="67"/>
+      <c r="E12" s="65" t="s">
         <v>195</v>
       </c>
-      <c r="F12" s="59"/>
+      <c r="F12" s="67"/>
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
       <c r="J12" s="13"/>
       <c r="K12" s="13"/>
       <c r="L12" s="13"/>
-      <c r="M12" s="57" t="s">
+      <c r="M12" s="65" t="s">
         <v>321</v>
       </c>
-      <c r="N12" s="59"/>
+      <c r="N12" s="67"/>
     </row>
     <row r="13" spans="1:14" ht="73.2" customHeight="1" thickBot="1">
-      <c r="A13" s="56"/>
+      <c r="A13" s="64"/>
       <c r="B13" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="C13" s="51" t="s">
+      <c r="C13" s="59" t="s">
         <v>196</v>
       </c>
-      <c r="D13" s="52"/>
+      <c r="D13" s="60"/>
       <c r="E13" s="22"/>
       <c r="F13" s="22"/>
       <c r="G13" s="22"/>
@@ -8074,7 +8074,7 @@
       <c r="N13" s="23"/>
     </row>
     <row r="14" spans="1:14" ht="100.2" customHeight="1">
-      <c r="A14" s="54" t="s">
+      <c r="A14" s="62" t="s">
         <v>145</v>
       </c>
       <c r="B14" s="17" t="s">
@@ -8088,10 +8088,10 @@
       <c r="F14" s="20" t="s">
         <v>198</v>
       </c>
-      <c r="G14" s="62" t="s">
+      <c r="G14" s="70" t="s">
         <v>199</v>
       </c>
-      <c r="H14" s="64"/>
+      <c r="H14" s="72"/>
       <c r="I14" s="20" t="s">
         <v>200</v>
       </c>
@@ -8104,7 +8104,7 @@
       <c r="N14" s="18"/>
     </row>
     <row r="15" spans="1:14" ht="156" customHeight="1">
-      <c r="A15" s="55"/>
+      <c r="A15" s="63"/>
       <c r="B15" s="10" t="s">
         <v>95</v>
       </c>
@@ -8118,10 +8118,10 @@
       <c r="F15" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="G15" s="57" t="s">
+      <c r="G15" s="65" t="s">
         <v>199</v>
       </c>
-      <c r="H15" s="59"/>
+      <c r="H15" s="67"/>
       <c r="I15" s="13" t="s">
         <v>200</v>
       </c>
@@ -8138,7 +8138,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" ht="147.6" customHeight="1">
-      <c r="A16" s="55"/>
+      <c r="A16" s="63"/>
       <c r="B16" s="10" t="s">
         <v>100</v>
       </c>
@@ -8154,10 +8154,10 @@
       <c r="F16" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="G16" s="57" t="s">
+      <c r="G16" s="65" t="s">
         <v>208</v>
       </c>
-      <c r="H16" s="59"/>
+      <c r="H16" s="67"/>
       <c r="I16" s="13" t="s">
         <v>209</v>
       </c>
@@ -8178,7 +8178,7 @@
       </c>
     </row>
     <row r="17" spans="1:14" ht="132.6">
-      <c r="A17" s="55"/>
+      <c r="A17" s="63"/>
       <c r="B17" s="10" t="s">
         <v>101</v>
       </c>
@@ -8190,10 +8190,10 @@
       <c r="F17" s="13" t="s">
         <v>214</v>
       </c>
-      <c r="G17" s="57" t="s">
+      <c r="G17" s="65" t="s">
         <v>208</v>
       </c>
-      <c r="H17" s="59"/>
+      <c r="H17" s="67"/>
       <c r="I17" s="13" t="s">
         <v>209</v>
       </c>
@@ -8212,7 +8212,7 @@
       </c>
     </row>
     <row r="18" spans="1:14" ht="102.6" customHeight="1" thickBot="1">
-      <c r="A18" s="56"/>
+      <c r="A18" s="64"/>
       <c r="B18" s="19" t="s">
         <v>308</v>
       </c>
@@ -8234,7 +8234,7 @@
       <c r="N18" s="23"/>
     </row>
     <row r="19" spans="1:14" ht="83.4" customHeight="1">
-      <c r="A19" s="54" t="s">
+      <c r="A19" s="62" t="s">
         <v>160</v>
       </c>
       <c r="B19" s="17" t="s">
@@ -8258,22 +8258,22 @@
       </c>
     </row>
     <row r="20" spans="1:14" ht="94.2" customHeight="1">
-      <c r="A20" s="55"/>
+      <c r="A20" s="63"/>
       <c r="B20" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="C20" s="57" t="s">
+      <c r="C20" s="65" t="s">
         <v>219</v>
       </c>
-      <c r="D20" s="59"/>
-      <c r="E20" s="57" t="s">
+      <c r="D20" s="67"/>
+      <c r="E20" s="65" t="s">
         <v>220</v>
       </c>
-      <c r="F20" s="59"/>
-      <c r="G20" s="57" t="s">
+      <c r="F20" s="67"/>
+      <c r="G20" s="65" t="s">
         <v>221</v>
       </c>
-      <c r="H20" s="59"/>
+      <c r="H20" s="67"/>
       <c r="I20" s="13"/>
       <c r="J20" s="13"/>
       <c r="K20" s="13" t="s">
@@ -8282,28 +8282,28 @@
       <c r="L20" s="13" t="s">
         <v>223</v>
       </c>
-      <c r="M20" s="57" t="s">
+      <c r="M20" s="65" t="s">
         <v>224</v>
       </c>
-      <c r="N20" s="59"/>
+      <c r="N20" s="67"/>
     </row>
     <row r="21" spans="1:14" ht="87.6" customHeight="1">
-      <c r="A21" s="55"/>
+      <c r="A21" s="63"/>
       <c r="B21" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="C21" s="57" t="s">
+      <c r="C21" s="65" t="s">
         <v>219</v>
       </c>
-      <c r="D21" s="59"/>
-      <c r="E21" s="57" t="s">
+      <c r="D21" s="67"/>
+      <c r="E21" s="65" t="s">
         <v>220</v>
       </c>
-      <c r="F21" s="59"/>
-      <c r="G21" s="57" t="s">
+      <c r="F21" s="67"/>
+      <c r="G21" s="65" t="s">
         <v>221</v>
       </c>
-      <c r="H21" s="59"/>
+      <c r="H21" s="67"/>
       <c r="I21" s="13"/>
       <c r="J21" s="13"/>
       <c r="K21" s="13" t="s">
@@ -8312,13 +8312,13 @@
       <c r="L21" s="13" t="s">
         <v>223</v>
       </c>
-      <c r="M21" s="57" t="s">
+      <c r="M21" s="65" t="s">
         <v>224</v>
       </c>
-      <c r="N21" s="59"/>
+      <c r="N21" s="67"/>
     </row>
     <row r="22" spans="1:14" ht="82.8" customHeight="1">
-      <c r="A22" s="55"/>
+      <c r="A22" s="63"/>
       <c r="B22" s="10" t="s">
         <v>308</v>
       </c>
@@ -8336,7 +8336,7 @@
       <c r="N22" s="9"/>
     </row>
     <row r="23" spans="1:14" ht="102.6" customHeight="1" thickBot="1">
-      <c r="A23" s="56"/>
+      <c r="A23" s="64"/>
       <c r="B23" s="19" t="s">
         <v>309</v>
       </c>
@@ -8354,36 +8354,36 @@
       <c r="N23" s="23"/>
     </row>
     <row r="24" spans="1:14" ht="102.6" customHeight="1">
-      <c r="A24" s="54" t="s">
+      <c r="A24" s="62" t="s">
         <v>173</v>
       </c>
       <c r="B24" s="17" t="s">
         <v>87</v>
       </c>
       <c r="C24" s="20"/>
-      <c r="D24" s="87"/>
+      <c r="D24" s="50"/>
       <c r="E24" s="20"/>
       <c r="F24" s="20"/>
       <c r="G24" s="90" t="s">
         <v>234</v>
       </c>
       <c r="H24" s="91"/>
-      <c r="I24" s="88"/>
-      <c r="J24" s="89"/>
-      <c r="K24" s="87"/>
+      <c r="I24" s="51"/>
+      <c r="J24" s="52"/>
+      <c r="K24" s="50"/>
       <c r="L24" s="20"/>
       <c r="M24" s="20"/>
       <c r="N24" s="18"/>
     </row>
     <row r="25" spans="1:14" ht="105" customHeight="1">
-      <c r="A25" s="80"/>
+      <c r="A25" s="88"/>
       <c r="B25" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="C25" s="82" t="s">
+      <c r="C25" s="85" t="s">
         <v>194</v>
       </c>
-      <c r="D25" s="83"/>
+      <c r="D25" s="87"/>
       <c r="E25" s="35" t="s">
         <v>228</v>
       </c>
@@ -8394,30 +8394,30 @@
         <v>234</v>
       </c>
       <c r="H25" s="91"/>
-      <c r="I25" s="82" t="s">
+      <c r="I25" s="85" t="s">
         <v>230</v>
       </c>
-      <c r="J25" s="84"/>
-      <c r="K25" s="83"/>
-      <c r="L25" s="85" t="s">
+      <c r="J25" s="86"/>
+      <c r="K25" s="87"/>
+      <c r="L25" s="48" t="s">
         <v>212</v>
       </c>
-      <c r="M25" s="86" t="s">
+      <c r="M25" s="49" t="s">
         <v>352</v>
       </c>
-      <c r="N25" s="86" t="s">
+      <c r="N25" s="49" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="87" customHeight="1">
-      <c r="A26" s="80"/>
+      <c r="A26" s="88"/>
       <c r="B26" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="C26" s="57" t="s">
+      <c r="C26" s="65" t="s">
         <v>194</v>
       </c>
-      <c r="D26" s="59"/>
+      <c r="D26" s="67"/>
       <c r="E26" s="13" t="s">
         <v>228</v>
       </c>
@@ -8426,11 +8426,11 @@
       </c>
       <c r="G26" s="35"/>
       <c r="H26" s="35"/>
-      <c r="I26" s="57" t="s">
+      <c r="I26" s="65" t="s">
         <v>232</v>
       </c>
-      <c r="J26" s="58"/>
-      <c r="K26" s="59"/>
+      <c r="J26" s="66"/>
+      <c r="K26" s="67"/>
       <c r="L26" s="13" t="s">
         <v>215</v>
       </c>
@@ -8442,7 +8442,7 @@
       </c>
     </row>
     <row r="27" spans="1:14" ht="89.4" customHeight="1">
-      <c r="A27" s="80"/>
+      <c r="A27" s="88"/>
       <c r="B27" s="10" t="s">
         <v>101</v>
       </c>
@@ -8457,12 +8457,12 @@
         <v>231</v>
       </c>
       <c r="G27" s="39"/>
-      <c r="H27" s="92"/>
-      <c r="I27" s="57" t="s">
+      <c r="H27" s="53"/>
+      <c r="I27" s="65" t="s">
         <v>232</v>
       </c>
-      <c r="J27" s="58"/>
-      <c r="K27" s="59"/>
+      <c r="J27" s="66"/>
+      <c r="K27" s="67"/>
       <c r="L27" s="13"/>
       <c r="M27" s="9" t="s">
         <v>353</v>
@@ -8470,7 +8470,7 @@
       <c r="N27" s="9"/>
     </row>
     <row r="28" spans="1:14" ht="83.4" customHeight="1" thickBot="1">
-      <c r="A28" s="81"/>
+      <c r="A28" s="89"/>
       <c r="B28" s="19" t="s">
         <v>308</v>
       </c>
@@ -8482,8 +8482,8 @@
         <v>233</v>
       </c>
       <c r="F28" s="22"/>
-      <c r="G28" s="94"/>
-      <c r="H28" s="93"/>
+      <c r="G28" s="55"/>
+      <c r="H28" s="54"/>
       <c r="I28" s="22"/>
       <c r="J28" s="22"/>
       <c r="K28" s="22"/>
@@ -8494,7 +8494,7 @@
       <c r="N28" s="23"/>
     </row>
     <row r="29" spans="1:14" ht="76.05" customHeight="1">
-      <c r="A29" s="54" t="s">
+      <c r="A29" s="62" t="s">
         <v>238</v>
       </c>
       <c r="B29" s="17" t="s">
@@ -8508,17 +8508,17 @@
       <c r="F29" s="20"/>
       <c r="G29" s="20"/>
       <c r="H29" s="20"/>
-      <c r="I29" s="62" t="s">
+      <c r="I29" s="70" t="s">
         <v>235</v>
       </c>
-      <c r="J29" s="63"/>
-      <c r="K29" s="64"/>
+      <c r="J29" s="71"/>
+      <c r="K29" s="72"/>
       <c r="L29" s="20"/>
       <c r="M29" s="20"/>
       <c r="N29" s="18"/>
     </row>
     <row r="30" spans="1:14" ht="75.599999999999994" customHeight="1" thickBot="1">
-      <c r="A30" s="56"/>
+      <c r="A30" s="64"/>
       <c r="B30" s="19" t="s">
         <v>237</v>
       </c>
@@ -8530,11 +8530,11 @@
       <c r="F30" s="22"/>
       <c r="G30" s="22"/>
       <c r="H30" s="22"/>
-      <c r="I30" s="51" t="s">
+      <c r="I30" s="59" t="s">
         <v>235</v>
       </c>
-      <c r="J30" s="53"/>
-      <c r="K30" s="52"/>
+      <c r="J30" s="61"/>
+      <c r="K30" s="60"/>
       <c r="L30" s="22"/>
       <c r="M30" s="22"/>
       <c r="N30" s="23"/>
@@ -8928,7 +8928,6 @@
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="A24:A28"/>
     <mergeCell ref="G24:H24"/>
     <mergeCell ref="G25:H25"/>
     <mergeCell ref="G1:H2"/>
@@ -8938,34 +8937,32 @@
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="E4:F4"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="C21:D21"/>
     <mergeCell ref="M4:N4"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="M5:N5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="M9:N9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:H10"/>
     <mergeCell ref="M10:N10"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="M11:N11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="G20:H20"/>
     <mergeCell ref="M12:N12"/>
     <mergeCell ref="G14:H14"/>
     <mergeCell ref="G15:H15"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="M20:N20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="G20:H20"/>
     <mergeCell ref="A9:A13"/>
     <mergeCell ref="I29:K29"/>
     <mergeCell ref="I30:K30"/>
@@ -8979,6 +8976,9 @@
     <mergeCell ref="A14:A18"/>
     <mergeCell ref="A19:A23"/>
     <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="A24:A28"/>
   </mergeCells>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="9" scale="31" orientation="landscape" r:id="rId1"/>
@@ -9011,40 +9011,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" ht="45" customHeight="1">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
       <c r="D1" s="30"/>
-      <c r="E1" s="71" t="s">
+      <c r="E1" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="75" t="s">
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="83" t="s">
         <v>351</v>
       </c>
-      <c r="I1" s="75"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
+      <c r="I1" s="83"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="92"/>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" ht="39" customHeight="1">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
       <c r="D2" s="31"/>
-      <c r="E2" s="74" t="s">
+      <c r="E2" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="93"/>
+      <c r="K2" s="93"/>
     </row>
     <row r="3" spans="1:11" s="2" customFormat="1" ht="26.25" customHeight="1" thickBot="1">
       <c r="A3" s="14" t="s">
@@ -9082,7 +9082,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="24" customHeight="1">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="62" t="s">
         <v>102</v>
       </c>
       <c r="B4" s="17" t="s">
@@ -9099,7 +9099,7 @@
       <c r="K4" s="18"/>
     </row>
     <row r="5" spans="1:11" ht="24" customHeight="1">
-      <c r="A5" s="55"/>
+      <c r="A5" s="63"/>
       <c r="B5" s="10" t="s">
         <v>95</v>
       </c>
@@ -9114,7 +9114,7 @@
       <c r="K5" s="9"/>
     </row>
     <row r="6" spans="1:11" ht="24" customHeight="1">
-      <c r="A6" s="55"/>
+      <c r="A6" s="63"/>
       <c r="B6" s="10" t="s">
         <v>100</v>
       </c>
@@ -9129,7 +9129,7 @@
       <c r="K6" s="9"/>
     </row>
     <row r="7" spans="1:11" ht="24" customHeight="1">
-      <c r="A7" s="55"/>
+      <c r="A7" s="63"/>
       <c r="B7" s="10" t="s">
         <v>101</v>
       </c>
@@ -9144,7 +9144,7 @@
       <c r="K7" s="9"/>
     </row>
     <row r="8" spans="1:11" ht="24" customHeight="1" thickBot="1">
-      <c r="A8" s="56"/>
+      <c r="A8" s="64"/>
       <c r="B8" s="19" t="s">
         <v>308</v>
       </c>
@@ -9159,7 +9159,7 @@
       <c r="K8" s="23"/>
     </row>
     <row r="9" spans="1:11" ht="24" customHeight="1">
-      <c r="A9" s="54" t="s">
+      <c r="A9" s="62" t="s">
         <v>123</v>
       </c>
       <c r="B9" s="17" t="s">
@@ -9176,7 +9176,7 @@
       <c r="K9" s="18"/>
     </row>
     <row r="10" spans="1:11" ht="24" customHeight="1">
-      <c r="A10" s="55"/>
+      <c r="A10" s="63"/>
       <c r="B10" s="10" t="s">
         <v>95</v>
       </c>
@@ -9191,7 +9191,7 @@
       <c r="K10" s="9"/>
     </row>
     <row r="11" spans="1:11" ht="24" customHeight="1">
-      <c r="A11" s="55"/>
+      <c r="A11" s="63"/>
       <c r="B11" s="10" t="s">
         <v>100</v>
       </c>
@@ -9206,7 +9206,7 @@
       <c r="K11" s="9"/>
     </row>
     <row r="12" spans="1:11" ht="24" customHeight="1">
-      <c r="A12" s="55"/>
+      <c r="A12" s="63"/>
       <c r="B12" s="10" t="s">
         <v>101</v>
       </c>
@@ -9221,7 +9221,7 @@
       <c r="K12" s="9"/>
     </row>
     <row r="13" spans="1:11" ht="24" customHeight="1" thickBot="1">
-      <c r="A13" s="56"/>
+      <c r="A13" s="64"/>
       <c r="B13" s="19" t="s">
         <v>308</v>
       </c>
@@ -9236,7 +9236,7 @@
       <c r="K13" s="23"/>
     </row>
     <row r="14" spans="1:11" ht="24" customHeight="1">
-      <c r="A14" s="54" t="s">
+      <c r="A14" s="62" t="s">
         <v>145</v>
       </c>
       <c r="B14" s="17" t="s">
@@ -9253,7 +9253,7 @@
       <c r="K14" s="18"/>
     </row>
     <row r="15" spans="1:11" ht="24" customHeight="1">
-      <c r="A15" s="55"/>
+      <c r="A15" s="63"/>
       <c r="B15" s="10" t="s">
         <v>95</v>
       </c>
@@ -9268,7 +9268,7 @@
       <c r="K15" s="9"/>
     </row>
     <row r="16" spans="1:11" ht="24" customHeight="1">
-      <c r="A16" s="55"/>
+      <c r="A16" s="63"/>
       <c r="B16" s="10" t="s">
         <v>100</v>
       </c>
@@ -9283,7 +9283,7 @@
       <c r="K16" s="9"/>
     </row>
     <row r="17" spans="1:11" ht="24" customHeight="1">
-      <c r="A17" s="55"/>
+      <c r="A17" s="63"/>
       <c r="B17" s="10" t="s">
         <v>101</v>
       </c>
@@ -9298,7 +9298,7 @@
       <c r="K17" s="9"/>
     </row>
     <row r="18" spans="1:11" ht="24" customHeight="1" thickBot="1">
-      <c r="A18" s="56"/>
+      <c r="A18" s="64"/>
       <c r="B18" s="19" t="s">
         <v>308</v>
       </c>
@@ -9313,7 +9313,7 @@
       <c r="K18" s="23"/>
     </row>
     <row r="19" spans="1:11" ht="24" customHeight="1">
-      <c r="A19" s="54" t="s">
+      <c r="A19" s="62" t="s">
         <v>160</v>
       </c>
       <c r="B19" s="17" t="s">
@@ -9330,7 +9330,7 @@
       <c r="K19" s="18"/>
     </row>
     <row r="20" spans="1:11" ht="24" customHeight="1">
-      <c r="A20" s="55"/>
+      <c r="A20" s="63"/>
       <c r="B20" s="10" t="s">
         <v>100</v>
       </c>
@@ -9345,7 +9345,7 @@
       <c r="K20" s="9"/>
     </row>
     <row r="21" spans="1:11" ht="24" customHeight="1">
-      <c r="A21" s="55"/>
+      <c r="A21" s="63"/>
       <c r="B21" s="10" t="s">
         <v>101</v>
       </c>
@@ -9360,57 +9360,57 @@
       <c r="K21" s="9"/>
     </row>
     <row r="22" spans="1:11" ht="82.8" customHeight="1" thickBot="1">
-      <c r="A22" s="55"/>
+      <c r="A22" s="63"/>
       <c r="B22" s="19" t="s">
         <v>308</v>
       </c>
       <c r="C22" s="12" t="s">
         <v>225</v>
       </c>
-      <c r="D22" s="60" t="s">
+      <c r="D22" s="68" t="s">
         <v>180</v>
       </c>
-      <c r="E22" s="61"/>
-      <c r="F22" s="60" t="s">
+      <c r="E22" s="69"/>
+      <c r="F22" s="68" t="s">
         <v>226</v>
       </c>
-      <c r="G22" s="61"/>
-      <c r="H22" s="60" t="s">
+      <c r="G22" s="69"/>
+      <c r="H22" s="68" t="s">
         <v>227</v>
       </c>
-      <c r="I22" s="61"/>
-      <c r="J22" s="60" t="s">
+      <c r="I22" s="69"/>
+      <c r="J22" s="68" t="s">
         <v>328</v>
       </c>
-      <c r="K22" s="61"/>
+      <c r="K22" s="69"/>
     </row>
     <row r="23" spans="1:11" ht="82.8" customHeight="1" thickBot="1">
-      <c r="A23" s="56"/>
+      <c r="A23" s="64"/>
       <c r="B23" s="19" t="s">
         <v>309</v>
       </c>
       <c r="C23" s="29" t="s">
         <v>225</v>
       </c>
-      <c r="D23" s="65" t="s">
+      <c r="D23" s="73" t="s">
         <v>180</v>
       </c>
-      <c r="E23" s="66"/>
-      <c r="F23" s="65" t="s">
+      <c r="E23" s="74"/>
+      <c r="F23" s="73" t="s">
         <v>226</v>
       </c>
-      <c r="G23" s="66"/>
-      <c r="H23" s="65" t="s">
+      <c r="G23" s="74"/>
+      <c r="H23" s="73" t="s">
         <v>227</v>
       </c>
-      <c r="I23" s="66"/>
-      <c r="J23" s="65" t="s">
+      <c r="I23" s="74"/>
+      <c r="J23" s="73" t="s">
         <v>328</v>
       </c>
-      <c r="K23" s="66"/>
+      <c r="K23" s="74"/>
     </row>
     <row r="24" spans="1:11" ht="31.2" customHeight="1">
-      <c r="A24" s="54" t="s">
+      <c r="A24" s="62" t="s">
         <v>173</v>
       </c>
       <c r="B24" s="17" t="s">
@@ -9427,7 +9427,7 @@
       <c r="K24" s="18"/>
     </row>
     <row r="25" spans="1:11" ht="31.2" customHeight="1">
-      <c r="A25" s="55"/>
+      <c r="A25" s="63"/>
       <c r="B25" s="10" t="s">
         <v>100</v>
       </c>
@@ -9442,7 +9442,7 @@
       <c r="K25" s="9"/>
     </row>
     <row r="26" spans="1:11" ht="31.2" customHeight="1">
-      <c r="A26" s="55"/>
+      <c r="A26" s="63"/>
       <c r="B26" s="10" t="s">
         <v>101</v>
       </c>
@@ -9457,7 +9457,7 @@
       <c r="K26" s="9"/>
     </row>
     <row r="27" spans="1:11" ht="31.2" customHeight="1" thickBot="1">
-      <c r="A27" s="56"/>
+      <c r="A27" s="64"/>
       <c r="B27" s="19" t="s">
         <v>308</v>
       </c>
@@ -9472,7 +9472,7 @@
       <c r="K27" s="23"/>
     </row>
     <row r="28" spans="1:11" ht="31.2" customHeight="1">
-      <c r="A28" s="54" t="s">
+      <c r="A28" s="62" t="s">
         <v>238</v>
       </c>
       <c r="B28" s="17" t="s">
@@ -9489,7 +9489,7 @@
       <c r="K28" s="18"/>
     </row>
     <row r="29" spans="1:11" ht="31.2" customHeight="1" thickBot="1">
-      <c r="A29" s="56"/>
+      <c r="A29" s="64"/>
       <c r="B29" s="19" t="s">
         <v>237</v>
       </c>
@@ -9736,7 +9736,6 @@
     <row r="56" spans="3:9" ht="30" customHeight="1"/>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A9:A13"/>
     <mergeCell ref="H1:I2"/>
     <mergeCell ref="A4:A8"/>
     <mergeCell ref="A1:C1"/>
@@ -9756,6 +9755,7 @@
     <mergeCell ref="J23:K23"/>
     <mergeCell ref="A19:A23"/>
     <mergeCell ref="A14:A18"/>
+    <mergeCell ref="A9:A13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="39" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -9780,20 +9780,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1" ht="45" customHeight="1">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="71" t="s">
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="75" t="s">
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="83" t="s">
         <v>351</v>
       </c>
-      <c r="H1" s="75"/>
+      <c r="H1" s="83"/>
       <c r="I1" s="30"/>
       <c r="J1" s="30"/>
       <c r="K1" s="30"/>
@@ -9803,18 +9803,18 @@
       <c r="O1" s="30"/>
     </row>
     <row r="2" spans="1:15" s="1" customFormat="1" ht="45.6" customHeight="1">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="80" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="74" t="s">
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
       <c r="I2" s="31"/>
       <c r="J2" s="31"/>
       <c r="K2" s="31"/>
@@ -9871,7 +9871,7 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="106.2" customHeight="1">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="62" t="s">
         <v>102</v>
       </c>
       <c r="B4" s="17" t="s">
@@ -9881,24 +9881,24 @@
       <c r="D4" s="20"/>
       <c r="E4" s="20"/>
       <c r="F4" s="20"/>
-      <c r="G4" s="62" t="s">
+      <c r="G4" s="70" t="s">
         <v>239</v>
       </c>
-      <c r="H4" s="63"/>
-      <c r="I4" s="64"/>
+      <c r="H4" s="71"/>
+      <c r="I4" s="72"/>
       <c r="J4" s="20"/>
       <c r="K4" s="20"/>
       <c r="L4" s="20"/>
       <c r="M4" s="38" t="s">
         <v>337</v>
       </c>
-      <c r="N4" s="67" t="s">
+      <c r="N4" s="75" t="s">
         <v>240</v>
       </c>
-      <c r="O4" s="68"/>
+      <c r="O4" s="76"/>
     </row>
     <row r="5" spans="1:15" ht="109.8" customHeight="1">
-      <c r="A5" s="55"/>
+      <c r="A5" s="63"/>
       <c r="B5" s="10" t="s">
         <v>95</v>
       </c>
@@ -9906,24 +9906,24 @@
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
-      <c r="G5" s="57" t="s">
+      <c r="G5" s="65" t="s">
         <v>239</v>
       </c>
-      <c r="H5" s="58"/>
-      <c r="I5" s="59"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="67"/>
       <c r="J5" s="13"/>
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
       <c r="M5" s="38" t="s">
         <v>337</v>
       </c>
-      <c r="N5" s="60" t="s">
+      <c r="N5" s="68" t="s">
         <v>241</v>
       </c>
-      <c r="O5" s="61"/>
+      <c r="O5" s="69"/>
     </row>
     <row r="6" spans="1:15" ht="94.2" customHeight="1">
-      <c r="A6" s="55"/>
+      <c r="A6" s="63"/>
       <c r="B6" s="10" t="s">
         <v>100</v>
       </c>
@@ -9931,26 +9931,26 @@
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
-      <c r="G6" s="57" t="s">
+      <c r="G6" s="65" t="s">
         <v>242</v>
       </c>
-      <c r="H6" s="58"/>
-      <c r="I6" s="59"/>
-      <c r="J6" s="57" t="s">
+      <c r="H6" s="66"/>
+      <c r="I6" s="67"/>
+      <c r="J6" s="65" t="s">
         <v>243</v>
       </c>
-      <c r="K6" s="58"/>
-      <c r="L6" s="59"/>
+      <c r="K6" s="66"/>
+      <c r="L6" s="67"/>
       <c r="M6" s="11" t="s">
         <v>244</v>
       </c>
-      <c r="N6" s="60" t="s">
+      <c r="N6" s="68" t="s">
         <v>241</v>
       </c>
-      <c r="O6" s="61"/>
+      <c r="O6" s="69"/>
     </row>
     <row r="7" spans="1:15" ht="129.6" customHeight="1" thickBot="1">
-      <c r="A7" s="56"/>
+      <c r="A7" s="64"/>
       <c r="B7" s="19" t="s">
         <v>101</v>
       </c>
@@ -9961,11 +9961,11 @@
       <c r="G7" s="22"/>
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
-      <c r="J7" s="51" t="s">
+      <c r="J7" s="59" t="s">
         <v>243</v>
       </c>
-      <c r="K7" s="53"/>
-      <c r="L7" s="52"/>
+      <c r="K7" s="61"/>
+      <c r="L7" s="60"/>
       <c r="M7" s="22" t="s">
         <v>245</v>
       </c>
@@ -9973,7 +9973,7 @@
       <c r="O7" s="23"/>
     </row>
     <row r="8" spans="1:15" ht="70.95" customHeight="1">
-      <c r="A8" s="54" t="s">
+      <c r="A8" s="62" t="s">
         <v>123</v>
       </c>
       <c r="B8" s="17" t="s">
@@ -9990,13 +9990,13 @@
       <c r="K8" s="20"/>
       <c r="L8" s="20"/>
       <c r="M8" s="20"/>
-      <c r="N8" s="67" t="s">
+      <c r="N8" s="75" t="s">
         <v>246</v>
       </c>
-      <c r="O8" s="68"/>
+      <c r="O8" s="76"/>
     </row>
     <row r="9" spans="1:15" ht="70.8" customHeight="1">
-      <c r="A9" s="55"/>
+      <c r="A9" s="63"/>
       <c r="B9" s="10" t="s">
         <v>100</v>
       </c>
@@ -10011,24 +10011,24 @@
       <c r="K9" s="13"/>
       <c r="L9" s="13"/>
       <c r="M9" s="13"/>
-      <c r="N9" s="60" t="s">
+      <c r="N9" s="68" t="s">
         <v>246</v>
       </c>
-      <c r="O9" s="61"/>
+      <c r="O9" s="69"/>
     </row>
     <row r="10" spans="1:15" ht="112.8" customHeight="1">
-      <c r="A10" s="55"/>
+      <c r="A10" s="63"/>
       <c r="B10" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="C10" s="57" t="s">
+      <c r="C10" s="65" t="s">
         <v>247</v>
       </c>
-      <c r="D10" s="59"/>
-      <c r="E10" s="57" t="s">
+      <c r="D10" s="67"/>
+      <c r="E10" s="65" t="s">
         <v>248</v>
       </c>
-      <c r="F10" s="59"/>
+      <c r="F10" s="67"/>
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
@@ -10038,24 +10038,24 @@
         <v>261</v>
       </c>
       <c r="M10" s="13"/>
-      <c r="N10" s="60" t="s">
+      <c r="N10" s="68" t="s">
         <v>246</v>
       </c>
-      <c r="O10" s="61"/>
+      <c r="O10" s="69"/>
     </row>
     <row r="11" spans="1:15" ht="75.599999999999994" customHeight="1" thickBot="1">
-      <c r="A11" s="56"/>
+      <c r="A11" s="64"/>
       <c r="B11" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="C11" s="51" t="s">
+      <c r="C11" s="59" t="s">
         <v>247</v>
       </c>
-      <c r="D11" s="52"/>
-      <c r="E11" s="51" t="s">
+      <c r="D11" s="60"/>
+      <c r="E11" s="59" t="s">
         <v>249</v>
       </c>
-      <c r="F11" s="52"/>
+      <c r="F11" s="60"/>
       <c r="G11" s="22"/>
       <c r="H11" s="22"/>
       <c r="I11" s="22"/>
@@ -10069,7 +10069,7 @@
       <c r="O11" s="23"/>
     </row>
     <row r="12" spans="1:15" ht="70.95" customHeight="1">
-      <c r="A12" s="54" t="s">
+      <c r="A12" s="62" t="s">
         <v>145</v>
       </c>
       <c r="B12" s="17" t="s">
@@ -10086,13 +10086,13 @@
       <c r="K12" s="20"/>
       <c r="L12" s="20"/>
       <c r="M12" s="20"/>
-      <c r="N12" s="67" t="s">
+      <c r="N12" s="75" t="s">
         <v>241</v>
       </c>
-      <c r="O12" s="68"/>
+      <c r="O12" s="76"/>
     </row>
     <row r="13" spans="1:15" ht="114" customHeight="1">
-      <c r="A13" s="55"/>
+      <c r="A13" s="63"/>
       <c r="B13" s="10" t="s">
         <v>100</v>
       </c>
@@ -10100,24 +10100,24 @@
       <c r="D13" s="13"/>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
-      <c r="G13" s="57" t="s">
+      <c r="G13" s="65" t="s">
         <v>250</v>
       </c>
-      <c r="H13" s="58"/>
-      <c r="I13" s="59"/>
+      <c r="H13" s="66"/>
+      <c r="I13" s="67"/>
       <c r="J13" s="13"/>
       <c r="K13" s="13"/>
       <c r="L13" s="13" t="s">
         <v>251</v>
       </c>
       <c r="M13" s="37"/>
-      <c r="N13" s="60" t="s">
+      <c r="N13" s="68" t="s">
         <v>241</v>
       </c>
-      <c r="O13" s="61"/>
+      <c r="O13" s="69"/>
     </row>
     <row r="14" spans="1:15" ht="109.2" customHeight="1">
-      <c r="A14" s="55"/>
+      <c r="A14" s="63"/>
       <c r="B14" s="10" t="s">
         <v>101</v>
       </c>
@@ -10125,24 +10125,24 @@
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
-      <c r="G14" s="57" t="s">
+      <c r="G14" s="65" t="s">
         <v>250</v>
       </c>
-      <c r="H14" s="58"/>
-      <c r="I14" s="59"/>
+      <c r="H14" s="66"/>
+      <c r="I14" s="67"/>
       <c r="J14" s="13"/>
       <c r="K14" s="13"/>
       <c r="L14" s="13" t="s">
         <v>251</v>
       </c>
       <c r="M14" s="36"/>
-      <c r="N14" s="60" t="s">
+      <c r="N14" s="68" t="s">
         <v>241</v>
       </c>
-      <c r="O14" s="61"/>
+      <c r="O14" s="69"/>
     </row>
     <row r="15" spans="1:15" ht="111" customHeight="1" thickBot="1">
-      <c r="A15" s="55"/>
+      <c r="A15" s="63"/>
       <c r="B15" s="19" t="s">
         <v>308</v>
       </c>
@@ -10160,7 +10160,7 @@
       <c r="O15" s="9"/>
     </row>
     <row r="16" spans="1:15" ht="88.2" customHeight="1">
-      <c r="A16" s="55"/>
+      <c r="A16" s="63"/>
       <c r="B16" s="10" t="s">
         <v>309</v>
       </c>
@@ -10179,16 +10179,16 @@
       <c r="O16" s="9"/>
     </row>
     <row r="17" spans="1:15" ht="78" customHeight="1">
-      <c r="A17" s="55"/>
+      <c r="A17" s="63"/>
       <c r="B17" s="10" t="s">
         <v>310</v>
       </c>
       <c r="C17" s="13"/>
       <c r="D17" s="13"/>
-      <c r="E17" s="57" t="s">
+      <c r="E17" s="65" t="s">
         <v>254</v>
       </c>
-      <c r="F17" s="59"/>
+      <c r="F17" s="67"/>
       <c r="G17" s="13"/>
       <c r="H17" s="13"/>
       <c r="I17" s="13"/>
@@ -10200,16 +10200,16 @@
       <c r="O17" s="9"/>
     </row>
     <row r="18" spans="1:15" ht="74.400000000000006" customHeight="1" thickBot="1">
-      <c r="A18" s="56"/>
+      <c r="A18" s="64"/>
       <c r="B18" s="19" t="s">
         <v>311</v>
       </c>
       <c r="C18" s="22"/>
       <c r="D18" s="22"/>
-      <c r="E18" s="51" t="s">
+      <c r="E18" s="59" t="s">
         <v>254</v>
       </c>
-      <c r="F18" s="52"/>
+      <c r="F18" s="60"/>
       <c r="G18" s="22"/>
       <c r="H18" s="22"/>
       <c r="I18" s="22"/>
@@ -10221,16 +10221,16 @@
       <c r="O18" s="23"/>
     </row>
     <row r="19" spans="1:15" ht="99.6" customHeight="1">
-      <c r="A19" s="54" t="s">
+      <c r="A19" s="62" t="s">
         <v>160</v>
       </c>
       <c r="B19" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="C19" s="62" t="s">
+      <c r="C19" s="70" t="s">
         <v>255</v>
       </c>
-      <c r="D19" s="64"/>
+      <c r="D19" s="72"/>
       <c r="E19" s="20"/>
       <c r="F19" s="20"/>
       <c r="G19" s="20"/>
@@ -10250,14 +10250,14 @@
       <c r="O19" s="18"/>
     </row>
     <row r="20" spans="1:15" ht="90" customHeight="1">
-      <c r="A20" s="55"/>
+      <c r="A20" s="63"/>
       <c r="B20" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="C20" s="57" t="s">
+      <c r="C20" s="65" t="s">
         <v>255</v>
       </c>
-      <c r="D20" s="59"/>
+      <c r="D20" s="67"/>
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
@@ -10277,16 +10277,16 @@
       <c r="O20" s="9"/>
     </row>
     <row r="21" spans="1:15" ht="125.4" customHeight="1">
-      <c r="A21" s="55"/>
+      <c r="A21" s="63"/>
       <c r="B21" s="10" t="s">
         <v>100</v>
       </c>
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
-      <c r="E21" s="57" t="s">
+      <c r="E21" s="65" t="s">
         <v>259</v>
       </c>
-      <c r="F21" s="59"/>
+      <c r="F21" s="67"/>
       <c r="G21" s="13" t="s">
         <v>260</v>
       </c>
@@ -10306,16 +10306,16 @@
       <c r="O21" s="9"/>
     </row>
     <row r="22" spans="1:15" ht="93" customHeight="1">
-      <c r="A22" s="55"/>
+      <c r="A22" s="63"/>
       <c r="B22" s="10" t="s">
         <v>101</v>
       </c>
       <c r="C22" s="13"/>
       <c r="D22" s="13"/>
-      <c r="E22" s="57" t="s">
+      <c r="E22" s="65" t="s">
         <v>259</v>
       </c>
-      <c r="F22" s="59"/>
+      <c r="F22" s="67"/>
       <c r="G22" s="13"/>
       <c r="H22" s="13" t="s">
         <v>260</v>
@@ -10333,7 +10333,7 @@
       <c r="O22" s="9"/>
     </row>
     <row r="23" spans="1:15" ht="82.2" customHeight="1" thickBot="1">
-      <c r="A23" s="56"/>
+      <c r="A23" s="64"/>
       <c r="B23" s="19" t="s">
         <v>308</v>
       </c>
@@ -10354,7 +10354,7 @@
       <c r="O23" s="23"/>
     </row>
     <row r="24" spans="1:15" ht="76.05" customHeight="1">
-      <c r="A24" s="54" t="s">
+      <c r="A24" s="62" t="s">
         <v>173</v>
       </c>
       <c r="B24" s="17" t="s">
@@ -10367,19 +10367,19 @@
       <c r="G24" s="20"/>
       <c r="H24" s="20"/>
       <c r="I24" s="20"/>
-      <c r="J24" s="62" t="s">
+      <c r="J24" s="70" t="s">
         <v>264</v>
       </c>
-      <c r="K24" s="63"/>
-      <c r="L24" s="64"/>
+      <c r="K24" s="71"/>
+      <c r="L24" s="72"/>
       <c r="M24" s="20"/>
-      <c r="N24" s="67" t="s">
+      <c r="N24" s="75" t="s">
         <v>265</v>
       </c>
-      <c r="O24" s="68"/>
+      <c r="O24" s="76"/>
     </row>
     <row r="25" spans="1:15" ht="112.8">
-      <c r="A25" s="55"/>
+      <c r="A25" s="63"/>
       <c r="B25" s="10" t="s">
         <v>95</v>
       </c>
@@ -10389,47 +10389,47 @@
         <v>266</v>
       </c>
       <c r="F25" s="13"/>
-      <c r="G25" s="57" t="s">
+      <c r="G25" s="65" t="s">
         <v>267</v>
       </c>
-      <c r="H25" s="58"/>
-      <c r="I25" s="59"/>
-      <c r="J25" s="57" t="s">
+      <c r="H25" s="66"/>
+      <c r="I25" s="67"/>
+      <c r="J25" s="65" t="s">
         <v>264</v>
       </c>
-      <c r="K25" s="58"/>
-      <c r="L25" s="59"/>
+      <c r="K25" s="66"/>
+      <c r="L25" s="67"/>
       <c r="M25" s="11" t="s">
         <v>268</v>
       </c>
-      <c r="N25" s="60" t="s">
+      <c r="N25" s="68" t="s">
         <v>265</v>
       </c>
-      <c r="O25" s="61"/>
+      <c r="O25" s="69"/>
     </row>
     <row r="26" spans="1:15" ht="112.8" customHeight="1">
-      <c r="A26" s="55"/>
+      <c r="A26" s="63"/>
       <c r="B26" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="C26" s="57" t="s">
+      <c r="C26" s="65" t="s">
         <v>269</v>
       </c>
-      <c r="D26" s="59"/>
-      <c r="E26" s="57" t="s">
+      <c r="D26" s="67"/>
+      <c r="E26" s="65" t="s">
         <v>270</v>
       </c>
-      <c r="F26" s="59"/>
-      <c r="G26" s="57" t="s">
+      <c r="F26" s="67"/>
+      <c r="G26" s="65" t="s">
         <v>271</v>
       </c>
-      <c r="H26" s="58"/>
-      <c r="I26" s="59"/>
-      <c r="J26" s="57" t="s">
+      <c r="H26" s="66"/>
+      <c r="I26" s="67"/>
+      <c r="J26" s="65" t="s">
         <v>272</v>
       </c>
-      <c r="K26" s="58"/>
-      <c r="L26" s="59"/>
+      <c r="K26" s="66"/>
+      <c r="L26" s="67"/>
       <c r="M26" s="13" t="s">
         <v>273</v>
       </c>
@@ -10437,14 +10437,14 @@
       <c r="O26" s="9"/>
     </row>
     <row r="27" spans="1:15" ht="129" customHeight="1">
-      <c r="A27" s="55"/>
+      <c r="A27" s="63"/>
       <c r="B27" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="C27" s="57" t="s">
+      <c r="C27" s="65" t="s">
         <v>269</v>
       </c>
-      <c r="D27" s="59"/>
+      <c r="D27" s="67"/>
       <c r="E27" s="13" t="s">
         <v>274</v>
       </c>
@@ -10454,19 +10454,19 @@
       <c r="G27" s="90" t="s">
         <v>271</v>
       </c>
-      <c r="H27" s="95"/>
+      <c r="H27" s="94"/>
       <c r="I27" s="91"/>
-      <c r="J27" s="57" t="s">
+      <c r="J27" s="65" t="s">
         <v>272</v>
       </c>
-      <c r="K27" s="58"/>
-      <c r="L27" s="59"/>
+      <c r="K27" s="66"/>
+      <c r="L27" s="67"/>
       <c r="M27" s="13"/>
       <c r="N27" s="9"/>
       <c r="O27" s="9"/>
     </row>
     <row r="28" spans="1:15" ht="73.8" customHeight="1" thickBot="1">
-      <c r="A28" s="56"/>
+      <c r="A28" s="64"/>
       <c r="B28" s="19" t="s">
         <v>308</v>
       </c>
@@ -10479,7 +10479,7 @@
       <c r="G28" s="90" t="s">
         <v>276</v>
       </c>
-      <c r="H28" s="95"/>
+      <c r="H28" s="94"/>
       <c r="I28" s="91"/>
       <c r="J28" s="22"/>
       <c r="K28" s="22"/>
@@ -10998,41 +10998,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" ht="45" customHeight="1">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
       <c r="D1" s="30"/>
-      <c r="E1" s="71" t="s">
+      <c r="E1" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="75" t="s">
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="83" t="s">
         <v>351</v>
       </c>
-      <c r="I1" s="75"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
+      <c r="I1" s="83"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="92"/>
       <c r="L1" s="32"/>
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" ht="45.6" customHeight="1">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="80" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
       <c r="D2" s="31"/>
-      <c r="E2" s="74" t="s">
+      <c r="E2" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="84"/>
+      <c r="I2" s="84"/>
+      <c r="J2" s="93"/>
+      <c r="K2" s="93"/>
       <c r="L2" s="33"/>
     </row>
     <row r="3" spans="1:12" s="2" customFormat="1" ht="26.25" customHeight="1" thickBot="1">
@@ -11074,7 +11074,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="23.4" customHeight="1">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="62" t="s">
         <v>102</v>
       </c>
       <c r="B4" s="17" t="s">
@@ -11092,7 +11092,7 @@
       <c r="L4" s="18"/>
     </row>
     <row r="5" spans="1:12" ht="23.4" customHeight="1">
-      <c r="A5" s="55"/>
+      <c r="A5" s="63"/>
       <c r="B5" s="10" t="s">
         <v>95</v>
       </c>
@@ -11108,7 +11108,7 @@
       <c r="L5" s="9"/>
     </row>
     <row r="6" spans="1:12" ht="23.4" customHeight="1">
-      <c r="A6" s="55"/>
+      <c r="A6" s="63"/>
       <c r="B6" s="10" t="s">
         <v>100</v>
       </c>
@@ -11124,7 +11124,7 @@
       <c r="L6" s="9"/>
     </row>
     <row r="7" spans="1:12" ht="23.4" customHeight="1" thickBot="1">
-      <c r="A7" s="56"/>
+      <c r="A7" s="64"/>
       <c r="B7" s="19" t="s">
         <v>101</v>
       </c>
@@ -11140,7 +11140,7 @@
       <c r="L7" s="23"/>
     </row>
     <row r="8" spans="1:12" ht="23.4" customHeight="1">
-      <c r="A8" s="54" t="s">
+      <c r="A8" s="62" t="s">
         <v>123</v>
       </c>
       <c r="B8" s="17" t="s">
@@ -11158,7 +11158,7 @@
       <c r="L8" s="18"/>
     </row>
     <row r="9" spans="1:12" ht="23.4" customHeight="1">
-      <c r="A9" s="55"/>
+      <c r="A9" s="63"/>
       <c r="B9" s="10" t="s">
         <v>100</v>
       </c>
@@ -11174,7 +11174,7 @@
       <c r="L9" s="9"/>
     </row>
     <row r="10" spans="1:12" ht="23.4" customHeight="1">
-      <c r="A10" s="55"/>
+      <c r="A10" s="63"/>
       <c r="B10" s="10" t="s">
         <v>101</v>
       </c>
@@ -11190,7 +11190,7 @@
       <c r="L10" s="9"/>
     </row>
     <row r="11" spans="1:12" ht="23.4" customHeight="1" thickBot="1">
-      <c r="A11" s="56"/>
+      <c r="A11" s="64"/>
       <c r="B11" s="19" t="s">
         <v>308</v>
       </c>
@@ -11206,7 +11206,7 @@
       <c r="L11" s="23"/>
     </row>
     <row r="12" spans="1:12" ht="23.4" customHeight="1">
-      <c r="A12" s="54" t="s">
+      <c r="A12" s="62" t="s">
         <v>145</v>
       </c>
       <c r="B12" s="17" t="s">
@@ -11224,7 +11224,7 @@
       <c r="L12" s="18"/>
     </row>
     <row r="13" spans="1:12" ht="23.4" customHeight="1">
-      <c r="A13" s="55"/>
+      <c r="A13" s="63"/>
       <c r="B13" s="10" t="s">
         <v>100</v>
       </c>
@@ -11240,7 +11240,7 @@
       <c r="L13" s="9"/>
     </row>
     <row r="14" spans="1:12" ht="23.4" customHeight="1">
-      <c r="A14" s="55"/>
+      <c r="A14" s="63"/>
       <c r="B14" s="10" t="s">
         <v>101</v>
       </c>
@@ -11256,59 +11256,59 @@
       <c r="L14" s="9"/>
     </row>
     <row r="15" spans="1:12" ht="88.2" customHeight="1">
-      <c r="A15" s="55"/>
+      <c r="A15" s="63"/>
       <c r="B15" s="10" t="s">
         <v>308</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>252</v>
       </c>
-      <c r="D15" s="60" t="s">
+      <c r="D15" s="68" t="s">
         <v>253</v>
       </c>
-      <c r="E15" s="79"/>
-      <c r="F15" s="61"/>
-      <c r="G15" s="60" t="s">
+      <c r="E15" s="95"/>
+      <c r="F15" s="69"/>
+      <c r="G15" s="68" t="s">
         <v>338</v>
       </c>
-      <c r="H15" s="61"/>
-      <c r="I15" s="60" t="s">
+      <c r="H15" s="69"/>
+      <c r="I15" s="68" t="s">
         <v>331</v>
       </c>
-      <c r="J15" s="61"/>
-      <c r="K15" s="60" t="s">
+      <c r="J15" s="69"/>
+      <c r="K15" s="68" t="s">
         <v>332</v>
       </c>
-      <c r="L15" s="61"/>
+      <c r="L15" s="69"/>
     </row>
     <row r="16" spans="1:12" ht="88.2" customHeight="1">
-      <c r="A16" s="55"/>
+      <c r="A16" s="63"/>
       <c r="B16" s="34" t="s">
         <v>309</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>252</v>
       </c>
-      <c r="D16" s="60" t="s">
+      <c r="D16" s="68" t="s">
         <v>253</v>
       </c>
-      <c r="E16" s="79"/>
-      <c r="F16" s="61"/>
-      <c r="G16" s="60" t="s">
+      <c r="E16" s="95"/>
+      <c r="F16" s="69"/>
+      <c r="G16" s="68" t="s">
         <v>338</v>
       </c>
-      <c r="H16" s="61"/>
-      <c r="I16" s="60" t="s">
+      <c r="H16" s="69"/>
+      <c r="I16" s="68" t="s">
         <v>331</v>
       </c>
-      <c r="J16" s="61"/>
-      <c r="K16" s="60" t="s">
+      <c r="J16" s="69"/>
+      <c r="K16" s="68" t="s">
         <v>332</v>
       </c>
-      <c r="L16" s="61"/>
+      <c r="L16" s="69"/>
     </row>
     <row r="17" spans="1:12" ht="21" customHeight="1">
-      <c r="A17" s="55"/>
+      <c r="A17" s="63"/>
       <c r="B17" s="10" t="s">
         <v>310</v>
       </c>
@@ -11324,7 +11324,7 @@
       <c r="L17" s="9"/>
     </row>
     <row r="18" spans="1:12" ht="21" customHeight="1" thickBot="1">
-      <c r="A18" s="56"/>
+      <c r="A18" s="64"/>
       <c r="B18" s="19" t="s">
         <v>311</v>
       </c>
@@ -11340,7 +11340,7 @@
       <c r="L18" s="23"/>
     </row>
     <row r="19" spans="1:12" ht="21" customHeight="1">
-      <c r="A19" s="54" t="s">
+      <c r="A19" s="62" t="s">
         <v>160</v>
       </c>
       <c r="B19" s="17" t="s">
@@ -11358,7 +11358,7 @@
       <c r="L19" s="18"/>
     </row>
     <row r="20" spans="1:12" ht="21" customHeight="1">
-      <c r="A20" s="55"/>
+      <c r="A20" s="63"/>
       <c r="B20" s="10" t="s">
         <v>95</v>
       </c>
@@ -11374,7 +11374,7 @@
       <c r="L20" s="9"/>
     </row>
     <row r="21" spans="1:12" ht="21" customHeight="1">
-      <c r="A21" s="55"/>
+      <c r="A21" s="63"/>
       <c r="B21" s="10" t="s">
         <v>100</v>
       </c>
@@ -11390,7 +11390,7 @@
       <c r="L21" s="9"/>
     </row>
     <row r="22" spans="1:12" ht="21" customHeight="1">
-      <c r="A22" s="55"/>
+      <c r="A22" s="63"/>
       <c r="B22" s="10" t="s">
         <v>101</v>
       </c>
@@ -11406,7 +11406,7 @@
       <c r="L22" s="9"/>
     </row>
     <row r="23" spans="1:12" ht="21" customHeight="1" thickBot="1">
-      <c r="A23" s="56"/>
+      <c r="A23" s="64"/>
       <c r="B23" s="19" t="s">
         <v>308</v>
       </c>
@@ -11422,7 +11422,7 @@
       <c r="L23" s="23"/>
     </row>
     <row r="24" spans="1:12" ht="21" customHeight="1">
-      <c r="A24" s="54" t="s">
+      <c r="A24" s="62" t="s">
         <v>173</v>
       </c>
       <c r="B24" s="17" t="s">
@@ -11440,7 +11440,7 @@
       <c r="L24" s="18"/>
     </row>
     <row r="25" spans="1:12" ht="21" customHeight="1">
-      <c r="A25" s="55"/>
+      <c r="A25" s="63"/>
       <c r="B25" s="10" t="s">
         <v>95</v>
       </c>
@@ -11456,7 +11456,7 @@
       <c r="L25" s="9"/>
     </row>
     <row r="26" spans="1:12" ht="21" customHeight="1">
-      <c r="A26" s="55"/>
+      <c r="A26" s="63"/>
       <c r="B26" s="10" t="s">
         <v>100</v>
       </c>
@@ -11472,7 +11472,7 @@
       <c r="L26" s="9"/>
     </row>
     <row r="27" spans="1:12" ht="21" customHeight="1">
-      <c r="A27" s="55"/>
+      <c r="A27" s="63"/>
       <c r="B27" s="10" t="s">
         <v>101</v>
       </c>
@@ -11488,7 +11488,7 @@
       <c r="L27" s="9"/>
     </row>
     <row r="28" spans="1:12" ht="21" customHeight="1" thickBot="1">
-      <c r="A28" s="56"/>
+      <c r="A28" s="64"/>
       <c r="B28" s="19" t="s">
         <v>308</v>
       </c>
@@ -11750,7 +11750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
@@ -11764,20 +11764,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="1" customFormat="1" ht="45" customHeight="1">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="71" t="s">
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="75" t="s">
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="83" t="s">
         <v>351</v>
       </c>
-      <c r="H1" s="75"/>
+      <c r="H1" s="83"/>
       <c r="I1" s="30"/>
       <c r="J1" s="30"/>
       <c r="K1" s="30"/>
@@ -11787,18 +11787,18 @@
       <c r="O1" s="32"/>
     </row>
     <row r="2" spans="1:21" s="1" customFormat="1" ht="49.8" customHeight="1">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="80" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="74" t="s">
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="84"/>
       <c r="I2" s="31"/>
       <c r="J2" s="31"/>
       <c r="K2" s="31"/>
@@ -11861,7 +11861,7 @@
       <c r="U3" s="5"/>
     </row>
     <row r="4" spans="1:21" ht="89.4" customHeight="1">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="62" t="s">
         <v>102</v>
       </c>
       <c r="B4" s="17" t="s">
@@ -11869,18 +11869,18 @@
       </c>
       <c r="C4" s="20"/>
       <c r="D4" s="20"/>
-      <c r="E4" s="62" t="s">
+      <c r="E4" s="70" t="s">
         <v>278</v>
       </c>
-      <c r="F4" s="64"/>
+      <c r="F4" s="72"/>
       <c r="G4" s="20"/>
       <c r="H4" s="20"/>
       <c r="I4" s="20"/>
-      <c r="J4" s="62" t="s">
+      <c r="J4" s="70" t="s">
         <v>279</v>
       </c>
-      <c r="K4" s="63"/>
-      <c r="L4" s="64"/>
+      <c r="K4" s="71"/>
+      <c r="L4" s="72"/>
       <c r="M4" s="20"/>
       <c r="N4" s="18"/>
       <c r="O4" s="18"/>
@@ -11892,24 +11892,24 @@
       <c r="U4" s="5"/>
     </row>
     <row r="5" spans="1:21" ht="80.400000000000006" customHeight="1">
-      <c r="A5" s="55"/>
+      <c r="A5" s="63"/>
       <c r="B5" s="10" t="s">
         <v>95</v>
       </c>
       <c r="C5" s="13"/>
       <c r="D5" s="13"/>
-      <c r="E5" s="57" t="s">
+      <c r="E5" s="65" t="s">
         <v>280</v>
       </c>
-      <c r="F5" s="59"/>
+      <c r="F5" s="67"/>
       <c r="G5" s="13"/>
       <c r="H5" s="13"/>
       <c r="I5" s="13"/>
-      <c r="J5" s="57" t="s">
+      <c r="J5" s="65" t="s">
         <v>279</v>
       </c>
-      <c r="K5" s="58"/>
-      <c r="L5" s="59"/>
+      <c r="K5" s="66"/>
+      <c r="L5" s="67"/>
       <c r="M5" s="13"/>
       <c r="N5" s="9"/>
       <c r="O5" s="9"/>
@@ -11921,16 +11921,16 @@
       <c r="U5" s="5"/>
     </row>
     <row r="6" spans="1:21" ht="130.19999999999999" customHeight="1">
-      <c r="A6" s="55"/>
+      <c r="A6" s="63"/>
       <c r="B6" s="10" t="s">
         <v>100</v>
       </c>
       <c r="C6" s="13"/>
       <c r="D6" s="13"/>
-      <c r="E6" s="57" t="s">
+      <c r="E6" s="65" t="s">
         <v>280</v>
       </c>
-      <c r="F6" s="59"/>
+      <c r="F6" s="67"/>
       <c r="G6" s="13"/>
       <c r="H6" s="13"/>
       <c r="I6" s="13"/>
@@ -11950,7 +11950,7 @@
       <c r="U6" s="5"/>
     </row>
     <row r="7" spans="1:21" ht="92.4" customHeight="1">
-      <c r="A7" s="55"/>
+      <c r="A7" s="63"/>
       <c r="B7" s="10" t="s">
         <v>101</v>
       </c>
@@ -11961,11 +11961,11 @@
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
       <c r="I7" s="13"/>
-      <c r="J7" s="57" t="s">
+      <c r="J7" s="65" t="s">
         <v>282</v>
       </c>
-      <c r="K7" s="58"/>
-      <c r="L7" s="59"/>
+      <c r="K7" s="66"/>
+      <c r="L7" s="67"/>
       <c r="M7" s="11" t="s">
         <v>283</v>
       </c>
@@ -11979,7 +11979,7 @@
       <c r="U7" s="5"/>
     </row>
     <row r="8" spans="1:21" ht="96" customHeight="1" thickBot="1">
-      <c r="A8" s="56"/>
+      <c r="A8" s="64"/>
       <c r="B8" s="19" t="s">
         <v>308</v>
       </c>
@@ -12012,7 +12012,7 @@
       <c r="U8" s="5"/>
     </row>
     <row r="9" spans="1:21" ht="71.400000000000006" customHeight="1">
-      <c r="A9" s="54" t="s">
+      <c r="A9" s="62" t="s">
         <v>123</v>
       </c>
       <c r="B9" s="17" t="s">
@@ -12029,10 +12029,10 @@
       <c r="K9" s="20"/>
       <c r="L9" s="20"/>
       <c r="M9" s="20"/>
-      <c r="N9" s="67" t="s">
+      <c r="N9" s="75" t="s">
         <v>285</v>
       </c>
-      <c r="O9" s="68"/>
+      <c r="O9" s="76"/>
       <c r="P9" s="5"/>
       <c r="Q9" s="5"/>
       <c r="R9" s="5"/>
@@ -12041,7 +12041,7 @@
       <c r="U9" s="5"/>
     </row>
     <row r="10" spans="1:21" ht="76.2" customHeight="1">
-      <c r="A10" s="55"/>
+      <c r="A10" s="63"/>
       <c r="B10" s="10" t="s">
         <v>95</v>
       </c>
@@ -12052,16 +12052,16 @@
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
-      <c r="J10" s="57" t="s">
+      <c r="J10" s="65" t="s">
         <v>286</v>
       </c>
-      <c r="K10" s="58"/>
-      <c r="L10" s="59"/>
+      <c r="K10" s="66"/>
+      <c r="L10" s="67"/>
       <c r="M10" s="13"/>
-      <c r="N10" s="60" t="s">
+      <c r="N10" s="68" t="s">
         <v>285</v>
       </c>
-      <c r="O10" s="61"/>
+      <c r="O10" s="69"/>
       <c r="P10" s="5"/>
       <c r="Q10" s="5"/>
       <c r="R10" s="5"/>
@@ -12070,7 +12070,7 @@
       <c r="U10" s="5"/>
     </row>
     <row r="11" spans="1:21" ht="73.2" customHeight="1">
-      <c r="A11" s="55"/>
+      <c r="A11" s="63"/>
       <c r="B11" s="10" t="s">
         <v>100</v>
       </c>
@@ -12081,11 +12081,11 @@
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
       <c r="I11" s="13"/>
-      <c r="J11" s="57" t="s">
+      <c r="J11" s="65" t="s">
         <v>286</v>
       </c>
-      <c r="K11" s="58"/>
-      <c r="L11" s="59"/>
+      <c r="K11" s="66"/>
+      <c r="L11" s="67"/>
       <c r="M11" s="13"/>
       <c r="N11" s="9"/>
       <c r="O11" s="9"/>
@@ -12097,7 +12097,7 @@
       <c r="U11" s="5"/>
     </row>
     <row r="12" spans="1:21" ht="73.8" customHeight="1">
-      <c r="A12" s="55"/>
+      <c r="A12" s="63"/>
       <c r="B12" s="10" t="s">
         <v>101</v>
       </c>
@@ -12108,11 +12108,11 @@
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
-      <c r="J12" s="57" t="s">
+      <c r="J12" s="65" t="s">
         <v>322</v>
       </c>
-      <c r="K12" s="58"/>
-      <c r="L12" s="59"/>
+      <c r="K12" s="66"/>
+      <c r="L12" s="67"/>
       <c r="M12" s="13"/>
       <c r="N12" s="9"/>
       <c r="O12" s="9"/>
@@ -12124,7 +12124,7 @@
       <c r="U12" s="5"/>
     </row>
     <row r="13" spans="1:21" ht="81" customHeight="1" thickBot="1">
-      <c r="A13" s="56"/>
+      <c r="A13" s="64"/>
       <c r="B13" s="19" t="s">
         <v>308</v>
       </c>
@@ -12135,11 +12135,11 @@
       <c r="G13" s="22"/>
       <c r="H13" s="22"/>
       <c r="I13" s="22"/>
-      <c r="J13" s="51" t="s">
+      <c r="J13" s="59" t="s">
         <v>287</v>
       </c>
-      <c r="K13" s="53"/>
-      <c r="L13" s="52"/>
+      <c r="K13" s="61"/>
+      <c r="L13" s="60"/>
       <c r="M13" s="22"/>
       <c r="N13" s="23"/>
       <c r="O13" s="23"/>
@@ -12151,7 +12151,7 @@
       <c r="U13" s="5"/>
     </row>
     <row r="14" spans="1:21" ht="76.2" customHeight="1">
-      <c r="A14" s="54" t="s">
+      <c r="A14" s="62" t="s">
         <v>145</v>
       </c>
       <c r="B14" s="17" t="s">
@@ -12182,7 +12182,7 @@
       <c r="U14" s="5"/>
     </row>
     <row r="15" spans="1:21" ht="70.8" customHeight="1">
-      <c r="A15" s="55"/>
+      <c r="A15" s="63"/>
       <c r="B15" s="10" t="s">
         <v>95</v>
       </c>
@@ -12190,11 +12190,11 @@
       <c r="D15" s="13"/>
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
-      <c r="G15" s="57" t="s">
+      <c r="G15" s="65" t="s">
         <v>290</v>
       </c>
-      <c r="H15" s="58"/>
-      <c r="I15" s="59"/>
+      <c r="H15" s="66"/>
+      <c r="I15" s="67"/>
       <c r="J15" s="13" t="s">
         <v>288</v>
       </c>
@@ -12203,10 +12203,10 @@
       </c>
       <c r="L15" s="13"/>
       <c r="M15" s="13"/>
-      <c r="N15" s="60" t="s">
+      <c r="N15" s="68" t="s">
         <v>292</v>
       </c>
-      <c r="O15" s="61"/>
+      <c r="O15" s="69"/>
       <c r="P15" s="5"/>
       <c r="Q15" s="5"/>
       <c r="R15" s="5"/>
@@ -12215,7 +12215,7 @@
       <c r="U15" s="5"/>
     </row>
     <row r="16" spans="1:21" ht="70.8" customHeight="1">
-      <c r="A16" s="55"/>
+      <c r="A16" s="63"/>
       <c r="B16" s="10" t="s">
         <v>100</v>
       </c>
@@ -12223,11 +12223,11 @@
       <c r="D16" s="13"/>
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
-      <c r="G16" s="57" t="s">
+      <c r="G16" s="65" t="s">
         <v>290</v>
       </c>
-      <c r="H16" s="58"/>
-      <c r="I16" s="59"/>
+      <c r="H16" s="66"/>
+      <c r="I16" s="67"/>
       <c r="J16" s="13" t="s">
         <v>293</v>
       </c>
@@ -12236,10 +12236,10 @@
       </c>
       <c r="L16" s="13"/>
       <c r="M16" s="13"/>
-      <c r="N16" s="60" t="s">
+      <c r="N16" s="68" t="s">
         <v>292</v>
       </c>
-      <c r="O16" s="61"/>
+      <c r="O16" s="69"/>
       <c r="P16" s="5"/>
       <c r="Q16" s="5"/>
       <c r="R16" s="5"/>
@@ -12248,7 +12248,7 @@
       <c r="U16" s="5"/>
     </row>
     <row r="17" spans="1:21" ht="94.2" customHeight="1">
-      <c r="A17" s="55"/>
+      <c r="A17" s="63"/>
       <c r="B17" s="10" t="s">
         <v>101</v>
       </c>
@@ -12256,11 +12256,11 @@
       <c r="D17" s="13"/>
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
-      <c r="G17" s="57" t="s">
+      <c r="G17" s="65" t="s">
         <v>295</v>
       </c>
-      <c r="H17" s="58"/>
-      <c r="I17" s="59"/>
+      <c r="H17" s="66"/>
+      <c r="I17" s="67"/>
       <c r="J17" s="13"/>
       <c r="K17" s="13" t="s">
         <v>294</v>
@@ -12277,7 +12277,7 @@
       <c r="U17" s="5"/>
     </row>
     <row r="18" spans="1:21" ht="94.2" customHeight="1">
-      <c r="A18" s="55"/>
+      <c r="A18" s="63"/>
       <c r="B18" s="10" t="s">
         <v>308</v>
       </c>
@@ -12285,11 +12285,11 @@
       <c r="D18" s="13"/>
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
-      <c r="G18" s="57" t="s">
+      <c r="G18" s="65" t="s">
         <v>295</v>
       </c>
-      <c r="H18" s="58"/>
-      <c r="I18" s="59"/>
+      <c r="H18" s="66"/>
+      <c r="I18" s="67"/>
       <c r="J18" s="13"/>
       <c r="K18" s="13"/>
       <c r="L18" s="13"/>
@@ -12304,7 +12304,7 @@
       <c r="U18" s="5"/>
     </row>
     <row r="19" spans="1:21" ht="55.2">
-      <c r="A19" s="55"/>
+      <c r="A19" s="63"/>
       <c r="B19" s="34" t="s">
         <v>309</v>
       </c>
@@ -12329,16 +12329,16 @@
       <c r="U19" s="5"/>
     </row>
     <row r="20" spans="1:21" ht="78" customHeight="1">
-      <c r="A20" s="55"/>
+      <c r="A20" s="63"/>
       <c r="B20" s="10" t="s">
         <v>310</v>
       </c>
-      <c r="C20" s="57" t="s">
+      <c r="C20" s="65" t="s">
         <v>254</v>
       </c>
-      <c r="D20" s="58"/>
-      <c r="E20" s="58"/>
-      <c r="F20" s="59"/>
+      <c r="D20" s="66"/>
+      <c r="E20" s="66"/>
+      <c r="F20" s="67"/>
       <c r="G20" s="13"/>
       <c r="H20" s="13"/>
       <c r="I20" s="13"/>
@@ -12356,16 +12356,16 @@
       <c r="U20" s="5"/>
     </row>
     <row r="21" spans="1:21" ht="85.2" customHeight="1" thickBot="1">
-      <c r="A21" s="56"/>
+      <c r="A21" s="64"/>
       <c r="B21" s="19" t="s">
         <v>311</v>
       </c>
-      <c r="C21" s="51" t="s">
+      <c r="C21" s="59" t="s">
         <v>254</v>
       </c>
-      <c r="D21" s="53"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="52"/>
+      <c r="D21" s="61"/>
+      <c r="E21" s="61"/>
+      <c r="F21" s="60"/>
       <c r="G21" s="22"/>
       <c r="H21" s="22"/>
       <c r="I21" s="22"/>
@@ -12383,7 +12383,7 @@
       <c r="U21" s="5"/>
     </row>
     <row r="22" spans="1:21" ht="84" customHeight="1">
-      <c r="A22" s="54" t="s">
+      <c r="A22" s="62" t="s">
         <v>160</v>
       </c>
       <c r="B22" s="17" t="s">
@@ -12396,10 +12396,10 @@
       <c r="G22" s="20"/>
       <c r="H22" s="20"/>
       <c r="I22" s="20"/>
-      <c r="J22" s="62" t="s">
+      <c r="J22" s="70" t="s">
         <v>296</v>
       </c>
-      <c r="K22" s="64"/>
+      <c r="K22" s="72"/>
       <c r="L22" s="20"/>
       <c r="M22" s="20"/>
       <c r="N22" s="18"/>
@@ -12412,7 +12412,7 @@
       <c r="U22" s="5"/>
     </row>
     <row r="23" spans="1:21" ht="131.4" customHeight="1">
-      <c r="A23" s="55"/>
+      <c r="A23" s="63"/>
       <c r="B23" s="10" t="s">
         <v>95</v>
       </c>
@@ -12420,15 +12420,15 @@
       <c r="D23" s="13"/>
       <c r="E23" s="13"/>
       <c r="F23" s="13"/>
-      <c r="G23" s="57" t="s">
+      <c r="G23" s="65" t="s">
         <v>297</v>
       </c>
-      <c r="H23" s="58"/>
-      <c r="I23" s="59"/>
-      <c r="J23" s="57" t="s">
+      <c r="H23" s="66"/>
+      <c r="I23" s="67"/>
+      <c r="J23" s="65" t="s">
         <v>296</v>
       </c>
-      <c r="K23" s="59"/>
+      <c r="K23" s="67"/>
       <c r="L23" s="13"/>
       <c r="M23" s="13" t="s">
         <v>263</v>
@@ -12443,7 +12443,7 @@
       <c r="U23" s="5"/>
     </row>
     <row r="24" spans="1:21" ht="105" customHeight="1">
-      <c r="A24" s="55"/>
+      <c r="A24" s="63"/>
       <c r="B24" s="10" t="s">
         <v>100</v>
       </c>
@@ -12478,7 +12478,7 @@
       <c r="U24" s="5"/>
     </row>
     <row r="25" spans="1:21" ht="106.8" customHeight="1">
-      <c r="A25" s="55"/>
+      <c r="A25" s="63"/>
       <c r="B25" s="10" t="s">
         <v>101</v>
       </c>
@@ -12505,7 +12505,7 @@
       <c r="U25" s="5"/>
     </row>
     <row r="26" spans="1:21" ht="103.8" customHeight="1" thickBot="1">
-      <c r="A26" s="55"/>
+      <c r="A26" s="63"/>
       <c r="B26" s="19" t="s">
         <v>308</v>
       </c>
@@ -12532,7 +12532,7 @@
       <c r="U26" s="5"/>
     </row>
     <row r="27" spans="1:21" ht="110.4" customHeight="1" thickBot="1">
-      <c r="A27" s="56"/>
+      <c r="A27" s="64"/>
       <c r="B27" s="10" t="s">
         <v>309</v>
       </c>
@@ -12559,16 +12559,16 @@
       <c r="U27" s="5"/>
     </row>
     <row r="28" spans="1:21" ht="80.400000000000006" customHeight="1">
-      <c r="A28" s="54" t="s">
+      <c r="A28" s="62" t="s">
         <v>173</v>
       </c>
       <c r="B28" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="C28" s="62" t="s">
+      <c r="C28" s="70" t="s">
         <v>302</v>
       </c>
-      <c r="D28" s="64"/>
+      <c r="D28" s="72"/>
       <c r="E28" s="20"/>
       <c r="F28" s="20"/>
       <c r="G28" s="20"/>
@@ -12590,16 +12590,16 @@
       <c r="U28" s="5"/>
     </row>
     <row r="29" spans="1:21" ht="90.6" customHeight="1">
-      <c r="A29" s="55"/>
+      <c r="A29" s="63"/>
       <c r="B29" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="C29" s="57" t="s">
+      <c r="C29" s="65" t="s">
         <v>303</v>
       </c>
-      <c r="D29" s="58"/>
-      <c r="E29" s="58"/>
-      <c r="F29" s="59"/>
+      <c r="D29" s="66"/>
+      <c r="E29" s="66"/>
+      <c r="F29" s="67"/>
       <c r="G29" s="13"/>
       <c r="H29" s="13"/>
       <c r="I29" s="13"/>
@@ -12621,16 +12621,16 @@
       <c r="U29" s="5"/>
     </row>
     <row r="30" spans="1:21" ht="196.2" customHeight="1">
-      <c r="A30" s="55"/>
+      <c r="A30" s="63"/>
       <c r="B30" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="C30" s="57" t="s">
+      <c r="C30" s="65" t="s">
         <v>303</v>
       </c>
-      <c r="D30" s="58"/>
-      <c r="E30" s="58"/>
-      <c r="F30" s="59"/>
+      <c r="D30" s="66"/>
+      <c r="E30" s="66"/>
+      <c r="F30" s="67"/>
       <c r="G30" s="13"/>
       <c r="H30" s="13"/>
       <c r="I30" s="13"/>
@@ -12656,7 +12656,7 @@
       <c r="U30" s="5"/>
     </row>
     <row r="31" spans="1:21" ht="180" customHeight="1">
-      <c r="A31" s="55"/>
+      <c r="A31" s="63"/>
       <c r="B31" s="10" t="s">
         <v>101</v>
       </c>
@@ -12689,7 +12689,7 @@
       <c r="U31" s="5"/>
     </row>
     <row r="32" spans="1:21" ht="93.6" customHeight="1" thickBot="1">
-      <c r="A32" s="55"/>
+      <c r="A32" s="63"/>
       <c r="B32" s="19" t="s">
         <v>308</v>
       </c>
@@ -12716,7 +12716,7 @@
       <c r="U32" s="5"/>
     </row>
     <row r="33" spans="1:21" ht="99" customHeight="1" thickBot="1">
-      <c r="A33" s="56"/>
+      <c r="A33" s="64"/>
       <c r="B33" s="10" t="s">
         <v>309</v>
       </c>
@@ -12743,7 +12743,7 @@
       <c r="U33" s="5"/>
     </row>
     <row r="34" spans="1:21" ht="107.4" customHeight="1">
-      <c r="A34" s="54" t="s">
+      <c r="A34" s="62" t="s">
         <v>238</v>
       </c>
       <c r="B34" s="17" t="s">
@@ -12772,7 +12772,7 @@
       <c r="U34" s="5"/>
     </row>
     <row r="35" spans="1:21" ht="108" customHeight="1">
-      <c r="A35" s="55"/>
+      <c r="A35" s="63"/>
       <c r="B35" s="10" t="s">
         <v>237</v>
       </c>
@@ -12799,7 +12799,7 @@
       <c r="U35" s="5"/>
     </row>
     <row r="36" spans="1:21" ht="102.6" customHeight="1" thickBot="1">
-      <c r="A36" s="56"/>
+      <c r="A36" s="64"/>
       <c r="B36" s="19" t="s">
         <v>307</v>
       </c>

</xml_diff>